<commit_message>
finished code and TSCV
TSCV results are too large to push to GitHub but can be requested for
</commit_message>
<xml_diff>
--- a/Accuracy rMAE and rRMSE (Cross-Sectional).xlsx
+++ b/Accuracy rMAE and rRMSE (Cross-Sectional).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e00c848d2da39f20/Documents/3. Masters/Research/WindPowerForecasting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="433" documentId="8_{7CAE70F8-1326-4B7D-8A8A-809CD0BBBC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{061F7B28-3F2F-4E61-A516-6548086381A0}"/>
+  <xr:revisionPtr revIDLastSave="618" documentId="8_{7CAE70F8-1326-4B7D-8A8A-809CD0BBBC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE315F62-DB23-4EBD-A571-397ADAD2A642}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{4F6B620E-8A72-45CF-9D17-FD2A4C076D11}"/>
   </bookViews>
@@ -106,7 +106,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -160,12 +160,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -185,6 +186,1083 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>LR AvRelRMSE</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="6"/>
+              <c:pt idx="0">
+                <c:v>Unreconciled</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v> BU</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v> TD</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v> MO</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v> OLS</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v> MinT-Shr</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Sheet1!$M$8,Sheet1!$M$16,Sheet1!$M$24,Sheet1!$M$32,Sheet1!$M$40,Sheet1!$M$48)</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.96447067964771771</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.97352881698353588</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.95844563471779165</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96778385588480964</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9594888849411255</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.95530003781890815</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C4A2-4C2B-B295-FE65B603BC74}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>LR AvRelMAE</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="6"/>
+              <c:pt idx="0">
+                <c:v>Unreconciled</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v> BU</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v> TD</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v> MO</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v> OLS</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v> MinT-Shr</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Sheet1!$G$8,Sheet1!$G$16,Sheet1!$G$24,Sheet1!$G$32,Sheet1!$G$40,Sheet1!$G$48)</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.0309700880227557</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0523003384247165</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.013318754775725</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0374231946797037</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.018162697334678</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0147622801069813</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C4A2-4C2B-B295-FE65B603BC74}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>GB AvRelMAE</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>(Sheet1!$G$56,Sheet1!$G$64,Sheet1!$G$72,Sheet1!$G$80,Sheet1!$G$88,Sheet1!$G$96)</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.0364136160503963</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0462386157374075</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0313097689495503</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0393989347860288</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.027878895513928</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0241623255952825</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BB80-4A83-8FE5-9A5DEF2879F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>GB AvRelRMSE</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>(Sheet1!$M$56,Sheet1!$M$64,Sheet1!$M$72,Sheet1!$M$80,Sheet1!$M$88,Sheet1!$M$96)</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.97202028869485435</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.970999859137338</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.97547640164003047</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.97331949246072047</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.96997165432465027</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.96362270616725443</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BB80-4A83-8FE5-9A5DEF2879F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="51328416"/>
+        <c:axId val="51326336"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="51328416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="51326336"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="51326336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="51328416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96006A19-4C8D-9D82-874A-6B9F98716CDB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -486,28 +1564,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9C5127F-CD46-4E4E-96B7-010FB4E47685}">
   <dimension ref="A1:M96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="26.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" customWidth="1"/>
+    <col min="3" max="3" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" customWidth="1"/>
     <col min="5" max="5" width="12.26953125" customWidth="1"/>
     <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.26953125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.26953125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.26953125" customWidth="1"/>
     <col min="11" max="11" width="11.7265625" customWidth="1"/>
     <col min="12" max="12" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -526,7 +1604,7 @@
       <c r="L1" s="2"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="4"/>
+      <c r="A2" s="5"/>
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
@@ -539,7 +1617,7 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="4"/>
+      <c r="A3" s="5"/>
       <c r="D3" s="2">
         <v>2</v>
       </c>
@@ -566,7 +1644,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="4"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
@@ -574,17 +1652,17 @@
         <v>0</v>
       </c>
       <c r="D4" s="3">
-        <v>1.05154974370181</v>
+        <v>1.0592846977557699</v>
       </c>
       <c r="E4" s="3">
-        <v>1.0203650443894501</v>
+        <v>1.02963208908215</v>
       </c>
       <c r="F4" s="3">
-        <v>0.98747753130219995</v>
-      </c>
-      <c r="G4" s="3">
+        <v>1.01954223361298</v>
+      </c>
+      <c r="G4" s="4">
         <f>GEOMEAN(D4:F4)</f>
-        <v>1.0194616008021999</v>
+        <v>1.0360164776196741</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>5</v>
@@ -593,95 +1671,95 @@
         <v>0</v>
       </c>
       <c r="J4" s="3">
-        <v>0.98040096964708001</v>
+        <v>0.95786849255492901</v>
       </c>
       <c r="K4" s="3">
-        <v>0.97347207255197099</v>
+        <v>0.96231137817143597</v>
       </c>
       <c r="L4" s="3">
-        <v>0.95365096153906503</v>
-      </c>
-      <c r="M4" s="3">
+        <v>0.963744194627697</v>
+      </c>
+      <c r="M4" s="4">
         <f>GEOMEAN(J4:L4)</f>
-        <v>0.96910810697145133</v>
+        <v>0.96130476414365063</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" s="4"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="3">
-        <v>1.0474372715960401</v>
+        <v>1.0624669731016201</v>
       </c>
       <c r="E5" s="3">
-        <v>1.0194938432284799</v>
+        <v>1.0345983790967499</v>
       </c>
       <c r="F5" s="3">
-        <v>0.98773467220877198</v>
-      </c>
-      <c r="G5" s="3">
+        <v>1.02254900769569</v>
+      </c>
+      <c r="G5" s="4">
         <f t="shared" ref="G5:G7" si="0">GEOMEAN(D5:F5)</f>
-        <v>1.0179293658144672</v>
+        <v>1.0397376919401935</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J5" s="3">
-        <v>0.97963888230496099</v>
+        <v>0.97142227333357301</v>
       </c>
       <c r="K5" s="3">
-        <v>0.97869614093086599</v>
+        <v>0.97546497471058602</v>
       </c>
       <c r="L5" s="3">
-        <v>0.97910453574234202</v>
-      </c>
-      <c r="M5" s="3">
+        <v>0.97708035678514105</v>
+      </c>
+      <c r="M5" s="4">
         <f t="shared" ref="M5:M7" si="1">GEOMEAN(J5:L5)</f>
-        <v>0.97914644357175751</v>
+        <v>0.97465296092529352</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="4"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="1"/>
       <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="3">
-        <v>1.0475607497802999</v>
+        <v>1.0586499521530099</v>
       </c>
       <c r="E6" s="3">
-        <v>1.01840071383195</v>
+        <v>1.03327618887192</v>
       </c>
       <c r="F6" s="3">
-        <v>0.98215180869375496</v>
-      </c>
-      <c r="G6" s="3">
+        <v>1.0095656598473799</v>
+      </c>
+      <c r="G6" s="4">
         <f t="shared" si="0"/>
-        <v>1.0156845459770616</v>
+        <v>1.0336363912819944</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J6" s="3">
-        <v>0.97684245801630398</v>
+        <v>0.96913220142851997</v>
       </c>
       <c r="K6" s="3">
-        <v>0.97585017100094495</v>
+        <v>0.973162609996154</v>
       </c>
       <c r="L6" s="3">
-        <v>0.95532206729795099</v>
-      </c>
-      <c r="M6" s="3">
+        <v>0.961803590485517</v>
+      </c>
+      <c r="M6" s="4">
         <f t="shared" si="1"/>
-        <v>0.96928723504110392</v>
+        <v>0.96802136850832932</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="4"/>
+      <c r="A7" s="5"/>
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
         <v>3</v>
@@ -695,7 +1773,7 @@
       <c r="F7" s="3">
         <v>0.98580504083140097</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="4">
         <f t="shared" si="0"/>
         <v>1.0146727995991616</v>
       </c>
@@ -712,7 +1790,7 @@
       <c r="L7" s="3">
         <v>0.94109852318371801</v>
       </c>
-      <c r="M7" s="3">
+      <c r="M7" s="4">
         <f t="shared" si="1"/>
         <v>0.95402569622407141</v>
       </c>
@@ -721,44 +1799,44 @@
       <c r="C8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="4">
         <f>GEOMEAN(D4:D7)</f>
-        <v>1.046901468511737</v>
-      </c>
-      <c r="E8" s="3">
+        <v>1.0553382353283558</v>
+      </c>
+      <c r="E8" s="4">
         <f t="shared" ref="E8:F8" si="2">GEOMEAN(E4:E7)</f>
-        <v>1.0190369474787218</v>
-      </c>
-      <c r="F8" s="3">
+        <v>1.0288280184444196</v>
+      </c>
+      <c r="F8" s="4">
         <f t="shared" si="2"/>
-        <v>0.98578974109159434</v>
-      </c>
-      <c r="G8" s="3">
+        <v>1.0092615755018655</v>
+      </c>
+      <c r="G8" s="4">
         <f>GEOMEAN(G4:G7)</f>
-        <v>1.0169353508793983</v>
+        <v>1.0309700880227557</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="4">
         <f>GEOMEAN(J4:J7)</f>
-        <v>0.97444223169964594</v>
-      </c>
-      <c r="K8" s="3">
+        <v>0.96484326925716257</v>
+      </c>
+      <c r="K8" s="4">
         <f t="shared" ref="K8" si="3">GEOMEAN(K4:K7)</f>
-        <v>0.97200249761073332</v>
-      </c>
-      <c r="L8" s="3">
+        <v>0.96773607515230597</v>
+      </c>
+      <c r="L8" s="4">
         <f t="shared" ref="L8" si="4">GEOMEAN(L4:L7)</f>
-        <v>0.95719595305295924</v>
-      </c>
-      <c r="M8" s="3">
+        <v>0.96084511344619006</v>
+      </c>
+      <c r="M8" s="4">
         <f>GEOMEAN(M4:M7)</f>
-        <v>0.96785012569681894</v>
+        <v>0.96447067964771771</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -777,7 +1855,7 @@
       <c r="L9" s="2"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" s="4"/>
+      <c r="A10" s="5"/>
       <c r="D10" s="1" t="s">
         <v>4</v>
       </c>
@@ -790,7 +1868,7 @@
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" s="4"/>
+      <c r="A11" s="5"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2">
         <v>2</v>
@@ -818,7 +1896,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" s="4"/>
+      <c r="A12" s="5"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -826,17 +1904,17 @@
         <v>0</v>
       </c>
       <c r="D12" s="3">
-        <v>1.05154974370181</v>
+        <v>1.0592846977557699</v>
       </c>
       <c r="E12" s="3">
-        <v>1.0530191285572701</v>
+        <v>1.04685597001332</v>
       </c>
       <c r="F12" s="3">
-        <v>1.0784709007279301</v>
-      </c>
-      <c r="G12" s="3">
+        <v>1.08688523187883</v>
+      </c>
+      <c r="G12" s="4">
         <f>GEOMEAN(D12:F12)</f>
-        <v>1.0609416634083453</v>
+        <v>1.0642110732152528</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>5</v>
@@ -845,95 +1923,95 @@
         <v>0</v>
       </c>
       <c r="J12" s="3">
-        <v>0.98040096964708001</v>
+        <v>0.95786849255492901</v>
       </c>
       <c r="K12" s="3">
-        <v>0.98281221042435796</v>
+        <v>0.96598968370306104</v>
       </c>
       <c r="L12" s="3">
-        <v>0.98724496030962905</v>
-      </c>
-      <c r="M12" s="3">
+        <v>0.98561052417299899</v>
+      </c>
+      <c r="M12" s="4">
         <f>GEOMEAN(J12:L12)</f>
-        <v>0.98348196515698583</v>
+        <v>0.96975323318332907</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" s="4"/>
+      <c r="A13" s="5"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="3">
-        <v>1.0474372715960401</v>
+        <v>1.0624669731016201</v>
       </c>
       <c r="E13" s="3">
-        <v>1.0362959286637199</v>
+        <v>1.04790841458322</v>
       </c>
       <c r="F13" s="3">
-        <v>1.04701669774221</v>
-      </c>
-      <c r="G13" s="3">
+        <v>1.0752517632168599</v>
+      </c>
+      <c r="G13" s="4">
         <f t="shared" ref="G13:G15" si="5">GEOMEAN(D13:F13)</f>
-        <v>1.0435705335621397</v>
+        <v>1.0618169243800228</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J13" s="3">
-        <v>0.97963888230496099</v>
+        <v>0.97142227333357301</v>
       </c>
       <c r="K13" s="3">
-        <v>0.97998376405555998</v>
+        <v>0.98035084069364198</v>
       </c>
       <c r="L13" s="3">
-        <v>0.98710822683622401</v>
-      </c>
-      <c r="M13" s="3">
+        <v>1.0006159697182899</v>
+      </c>
+      <c r="M13" s="4">
         <f t="shared" ref="M13:M15" si="6">GEOMEAN(J13:L13)</f>
-        <v>0.98223760112746505</v>
+        <v>0.98405416576171734</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" s="4"/>
+      <c r="A14" s="5"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="3">
-        <v>1.0475607497802999</v>
+        <v>1.0586499521530099</v>
       </c>
       <c r="E14" s="3">
-        <v>1.0322562538725899</v>
+        <v>1.0438183109836101</v>
       </c>
       <c r="F14" s="3">
-        <v>1.0410670749398001</v>
-      </c>
-      <c r="G14" s="3">
+        <v>1.0587780829736999</v>
+      </c>
+      <c r="G14" s="4">
         <f t="shared" si="5"/>
-        <v>1.0402757723380389</v>
+        <v>1.0537253106790809</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J14" s="3">
-        <v>0.97684245801630398</v>
+        <v>0.96913220142851997</v>
       </c>
       <c r="K14" s="3">
-        <v>0.98216254379036805</v>
+        <v>0.977871288832728</v>
       </c>
       <c r="L14" s="3">
-        <v>0.98668613505540204</v>
-      </c>
-      <c r="M14" s="3">
+        <v>0.989730764897368</v>
+      </c>
+      <c r="M14" s="4">
         <f t="shared" si="6"/>
-        <v>0.98188880167741932</v>
+        <v>0.97887505889922799</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="4"/>
+      <c r="A15" s="5"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
         <v>3</v>
@@ -947,7 +2025,7 @@
       <c r="F15" s="3">
         <v>1.0232234443550099</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="4">
         <f t="shared" si="5"/>
         <v>1.0298026651788392</v>
       </c>
@@ -964,7 +2042,7 @@
       <c r="L15" s="3">
         <v>0.96073965805616801</v>
       </c>
-      <c r="M15" s="3">
+      <c r="M15" s="4">
         <f t="shared" si="6"/>
         <v>0.96158513739777274</v>
       </c>
@@ -973,44 +2051,44 @@
       <c r="C16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="4">
         <f>GEOMEAN(D12:D15)</f>
-        <v>1.046901468511737</v>
-      </c>
-      <c r="E16" s="3">
+        <v>1.0553382353283558</v>
+      </c>
+      <c r="E16" s="4">
         <f t="shared" ref="E16" si="7">GEOMEAN(E12:E15)</f>
-        <v>1.0366406588513635</v>
-      </c>
-      <c r="F16" s="3">
+        <v>1.0409027072709713</v>
+      </c>
+      <c r="F16" s="4">
         <f t="shared" ref="F16" si="8">GEOMEAN(F12:F15)</f>
-        <v>1.0472558819832838</v>
-      </c>
-      <c r="G16" s="3">
+        <v>1.0607604503742138</v>
+      </c>
+      <c r="G16" s="4">
         <f>GEOMEAN(G12:G15)</f>
-        <v>1.0435877005287166</v>
+        <v>1.0523003384247165</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="4">
         <f>GEOMEAN(J12:J15)</f>
-        <v>0.97444223169964594</v>
-      </c>
-      <c r="K16" s="3">
+        <v>0.96484326925716257</v>
+      </c>
+      <c r="K16" s="4">
         <f t="shared" ref="K16" si="9">GEOMEAN(K12:K15)</f>
-        <v>0.97695609279810225</v>
-      </c>
-      <c r="L16" s="3">
+        <v>0.97177511835524477</v>
+      </c>
+      <c r="L16" s="4">
         <f t="shared" ref="L16" si="10">GEOMEAN(L12:L15)</f>
-        <v>0.98037812001251246</v>
-      </c>
-      <c r="M16" s="3">
+        <v>0.98406523101753762</v>
+      </c>
+      <c r="M16" s="4">
         <f>GEOMEAN(M12:M15)</f>
-        <v>0.97725578775433208</v>
+        <v>0.97352881698353588</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1029,7 +2107,7 @@
       <c r="L17" s="2"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" s="4"/>
+      <c r="A18" s="5"/>
       <c r="D18" s="1" t="s">
         <v>4</v>
       </c>
@@ -1042,7 +2120,7 @@
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" s="4"/>
+      <c r="A19" s="5"/>
       <c r="D19" s="2">
         <v>2</v>
       </c>
@@ -1069,7 +2147,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20" s="4"/>
+      <c r="A20" s="5"/>
       <c r="B20" s="1" t="s">
         <v>5</v>
       </c>
@@ -1077,17 +2155,17 @@
         <v>0</v>
       </c>
       <c r="D20" s="3">
-        <v>1.01565308095687</v>
+        <v>1.0228197397981</v>
       </c>
       <c r="E20" s="3">
-        <v>1.00038376685246</v>
+        <v>1.00371689303388</v>
       </c>
       <c r="F20" s="3">
-        <v>0.98747753130219995</v>
-      </c>
-      <c r="G20" s="3">
+        <v>1.01954223361298</v>
+      </c>
+      <c r="G20" s="4">
         <f>GEOMEAN(D20:F20)</f>
-        <v>1.0011052746167066</v>
+        <v>1.0153252462482847</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>5</v>
@@ -1096,95 +2174,95 @@
         <v>0</v>
       </c>
       <c r="J20" s="3">
-        <v>0.97115785075932104</v>
+        <v>0.95144852670656799</v>
       </c>
       <c r="K20" s="3">
-        <v>0.96623489703755605</v>
+        <v>0.95429728578715001</v>
       </c>
       <c r="L20" s="3">
-        <v>0.95365096153906503</v>
-      </c>
-      <c r="M20" s="3">
+        <v>0.963744194627697</v>
+      </c>
+      <c r="M20" s="4">
         <f>GEOMEAN(J20:L20)</f>
-        <v>0.96365297163613195</v>
+        <v>0.95648226218687182</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A21" s="4"/>
+      <c r="A21" s="5"/>
       <c r="B21" s="1"/>
       <c r="C21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D21" s="3">
-        <v>1.0207036161879199</v>
+        <v>1.03210039427949</v>
       </c>
       <c r="E21" s="3">
-        <v>1.0017400034061199</v>
+        <v>1.0123622894270901</v>
       </c>
       <c r="F21" s="3">
-        <v>0.98773467220877198</v>
-      </c>
-      <c r="G21" s="3">
+        <v>1.02254900769569</v>
+      </c>
+      <c r="G21" s="4">
         <f t="shared" ref="G21:G23" si="11">GEOMEAN(D21:F21)</f>
-        <v>1.0033019504442571</v>
+        <v>1.0223054552264137</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J21" s="3">
-        <v>0.97853789262405699</v>
+        <v>0.963549379381616</v>
       </c>
       <c r="K21" s="3">
-        <v>0.97697533223897604</v>
+        <v>0.96741125401856098</v>
       </c>
       <c r="L21" s="3">
-        <v>0.97910453574234202</v>
-      </c>
-      <c r="M21" s="3">
+        <v>0.97708035678514105</v>
+      </c>
+      <c r="M21" s="4">
         <f t="shared" ref="M21:M23" si="12">GEOMEAN(J21:L21)</f>
-        <v>0.97820550569910214</v>
+        <v>0.96933032108217998</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A22" s="4"/>
+      <c r="A22" s="5"/>
       <c r="B22" s="1"/>
       <c r="C22" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D22" s="3">
-        <v>1.0155937368466601</v>
+        <v>1.0263982398206</v>
       </c>
       <c r="E22" s="3">
-        <v>0.99608231411995396</v>
+        <v>1.0100643019183599</v>
       </c>
       <c r="F22" s="3">
-        <v>0.98215180869375496</v>
-      </c>
-      <c r="G22" s="3">
+        <v>1.0095656598473799</v>
+      </c>
+      <c r="G22" s="4">
         <f t="shared" si="11"/>
-        <v>0.99784852858256523</v>
+        <v>1.0153127272489262</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J22" s="3">
-        <v>0.96725482719906797</v>
+        <v>0.95714153250074496</v>
       </c>
       <c r="K22" s="3">
-        <v>0.96532749178391597</v>
+        <v>0.96162661993674803</v>
       </c>
       <c r="L22" s="3">
-        <v>0.95532206729795099</v>
-      </c>
-      <c r="M22" s="3">
+        <v>0.961803590485517</v>
+      </c>
+      <c r="M22" s="4">
         <f t="shared" si="12"/>
-        <v>0.96262055300167315</v>
+        <v>0.96018815516243883</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A23" s="4"/>
+      <c r="A23" s="5"/>
       <c r="B23" s="1"/>
       <c r="C23" s="2" t="s">
         <v>3</v>
@@ -1198,7 +2276,7 @@
       <c r="F23" s="3">
         <v>0.98580504083140097</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23" s="4">
         <f t="shared" si="11"/>
         <v>1.0004574657383061</v>
       </c>
@@ -1215,7 +2293,7 @@
       <c r="L23" s="3">
         <v>0.94109852318371801</v>
       </c>
-      <c r="M23" s="3">
+      <c r="M23" s="4">
         <f t="shared" si="12"/>
         <v>0.94790512690806328</v>
       </c>
@@ -1224,44 +2302,44 @@
       <c r="C24" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="4">
         <f>GEOMEAN(D20:D23)</f>
-        <v>1.0167318084951298</v>
-      </c>
-      <c r="E24" s="3">
+        <v>1.0240575933317637</v>
+      </c>
+      <c r="E24" s="4">
         <f t="shared" ref="E24" si="13">GEOMEAN(E20:E23)</f>
-        <v>0.99974740992835387</v>
-      </c>
-      <c r="F24" s="3">
+        <v>1.0067233017144941</v>
+      </c>
+      <c r="F24" s="4">
         <f t="shared" ref="F24" si="14">GEOMEAN(F20:F23)</f>
-        <v>0.98578974109159434</v>
-      </c>
-      <c r="G24" s="3">
+        <v>1.0092615755018655</v>
+      </c>
+      <c r="G24" s="4">
         <f>GEOMEAN(G20:G23)</f>
-        <v>1.0006764154664956</v>
+        <v>1.013318754775725</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J24" s="3">
+      <c r="J24" s="4">
         <f>GEOMEAN(J20:J23)</f>
-        <v>0.96709620751798231</v>
-      </c>
-      <c r="K24" s="3">
+        <v>0.95593077713820407</v>
+      </c>
+      <c r="K24" s="4">
         <f t="shared" ref="K24" si="15">GEOMEAN(K20:K23)</f>
-        <v>0.96484498456666989</v>
-      </c>
-      <c r="L24" s="3">
+        <v>0.95856732498998409</v>
+      </c>
+      <c r="L24" s="4">
         <f t="shared" ref="L24" si="16">GEOMEAN(L20:L23)</f>
-        <v>0.95719595305295924</v>
-      </c>
-      <c r="M24" s="3">
+        <v>0.96084511344619006</v>
+      </c>
+      <c r="M24" s="4">
         <f>GEOMEAN(M20:M23)</f>
-        <v>0.96303637789208696</v>
+        <v>0.95844563471779165</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1280,7 +2358,7 @@
       <c r="L25" s="2"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A26" s="4"/>
+      <c r="A26" s="5"/>
       <c r="D26" s="1" t="s">
         <v>4</v>
       </c>
@@ -1293,7 +2371,7 @@
       <c r="L26" s="1"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A27" s="4"/>
+      <c r="A27" s="5"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2">
         <v>2</v>
@@ -1321,7 +2399,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A28" s="4"/>
+      <c r="A28" s="5"/>
       <c r="B28" s="1" t="s">
         <v>5</v>
       </c>
@@ -1329,17 +2407,17 @@
         <v>0</v>
       </c>
       <c r="D28" s="3">
-        <v>1.02866656805479</v>
+        <v>1.0451574791462701</v>
       </c>
       <c r="E28" s="3">
-        <v>1.0203650443894501</v>
+        <v>1.02963208908215</v>
       </c>
       <c r="F28" s="3">
-        <v>1.02021479091491</v>
-      </c>
-      <c r="G28" s="3">
+        <v>1.0564432832645301</v>
+      </c>
+      <c r="G28" s="4">
         <f>GEOMEAN(D28:F28)</f>
-        <v>1.0230745258375042</v>
+        <v>1.0436863320263041</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>5</v>
@@ -1348,95 +2426,95 @@
         <v>0</v>
       </c>
       <c r="J28" s="3">
-        <v>0.974418815904735</v>
+        <v>0.95540855624620002</v>
       </c>
       <c r="K28" s="3">
-        <v>0.97347207255197099</v>
+        <v>0.96231137817143597</v>
       </c>
       <c r="L28" s="3">
-        <v>0.96541691763732396</v>
-      </c>
-      <c r="M28" s="3">
+        <v>0.97507127672308302</v>
+      </c>
+      <c r="M28" s="4">
         <f>GEOMEAN(J28:L28)</f>
-        <v>0.97109418700767736</v>
+        <v>0.96422940197681983</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A29" s="4"/>
+      <c r="A29" s="5"/>
       <c r="B29" s="1"/>
       <c r="C29" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D29" s="3">
-        <v>1.0347425026645201</v>
+        <v>1.05071023730076</v>
       </c>
       <c r="E29" s="3">
-        <v>1.0194938432284799</v>
+        <v>1.0345983790967499</v>
       </c>
       <c r="F29" s="3">
-        <v>1.01597232298245</v>
-      </c>
-      <c r="G29" s="3">
+        <v>1.05262441781215</v>
+      </c>
+      <c r="G29" s="4">
         <f t="shared" ref="G29:G31" si="17">GEOMEAN(D29:F29)</f>
-        <v>1.0233705720549604</v>
+        <v>1.0459463270126135</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J29" s="3">
-        <v>0.97764498977137104</v>
+        <v>0.96840645966161498</v>
       </c>
       <c r="K29" s="3">
-        <v>0.97869614093086599</v>
+        <v>0.97546497471058602</v>
       </c>
       <c r="L29" s="3">
-        <v>0.98095564536580004</v>
-      </c>
-      <c r="M29" s="3">
+        <v>0.98858558669989005</v>
+      </c>
+      <c r="M29" s="4">
         <f t="shared" ref="M29:M31" si="18">GEOMEAN(J29:L29)</f>
-        <v>0.97909795144050404</v>
+        <v>0.97744998443858488</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A30" s="4"/>
+      <c r="A30" s="5"/>
       <c r="B30" s="1"/>
       <c r="C30" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D30" s="3">
-        <v>1.0353755818705099</v>
+        <v>1.0466996668292099</v>
       </c>
       <c r="E30" s="3">
-        <v>1.01840071383195</v>
+        <v>1.03327618887192</v>
       </c>
       <c r="F30" s="3">
-        <v>1.01485372847066</v>
-      </c>
-      <c r="G30" s="3">
+        <v>1.0394244447947101</v>
+      </c>
+      <c r="G30" s="4">
         <f t="shared" si="17"/>
-        <v>1.0228376090627551</v>
+        <v>1.0397856301903527</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J30" s="3">
-        <v>0.97328205039155802</v>
+        <v>0.96538583662063304</v>
       </c>
       <c r="K30" s="3">
-        <v>0.97585017100094495</v>
+        <v>0.973162609996154</v>
       </c>
       <c r="L30" s="3">
-        <v>0.970742519308743</v>
-      </c>
-      <c r="M30" s="3">
+        <v>0.97779508796447601</v>
+      </c>
+      <c r="M30" s="4">
         <f t="shared" si="18"/>
-        <v>0.97328934656064503</v>
+        <v>0.97210101413935612</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A31" s="4"/>
+      <c r="A31" s="5"/>
       <c r="B31" s="1"/>
       <c r="C31" s="2" t="s">
         <v>3</v>
@@ -1450,7 +2528,7 @@
       <c r="F31" s="3">
         <v>1.0104144699051001</v>
       </c>
-      <c r="G31" s="3">
+      <c r="G31" s="4">
         <f t="shared" si="17"/>
         <v>1.0204708615588414</v>
       </c>
@@ -1467,7 +2545,7 @@
       <c r="L31" s="3">
         <v>0.95321076020532602</v>
       </c>
-      <c r="M31" s="3">
+      <c r="M31" s="4">
         <f t="shared" si="18"/>
         <v>0.95747442442063202</v>
       </c>
@@ -1476,44 +2554,44 @@
       <c r="C32" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="4">
         <f>GEOMEAN(D28:D31)</f>
-        <v>1.0330029532829379</v>
-      </c>
-      <c r="E32" s="3">
+        <v>1.0439316161691148</v>
+      </c>
+      <c r="E32" s="4">
         <f t="shared" ref="E32" si="19">GEOMEAN(E28:E31)</f>
-        <v>1.0190369474787218</v>
-      </c>
-      <c r="F32" s="3">
+        <v>1.0288280184444196</v>
+      </c>
+      <c r="F32" s="4">
         <f t="shared" ref="F32" si="20">GEOMEAN(F28:F31)</f>
-        <v>1.0153578371783105</v>
-      </c>
-      <c r="G32" s="3">
+        <v>1.0395682988116564</v>
+      </c>
+      <c r="G32" s="4">
         <f>GEOMEAN(G28:G31)</f>
-        <v>1.0224377431394129</v>
+        <v>1.0374231946797037</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J32" s="3">
+      <c r="J32" s="4">
         <f>GEOMEAN(J28:J31)</f>
-        <v>0.9710929229565235</v>
-      </c>
-      <c r="K32" s="3">
+        <v>0.96206924651663372</v>
+      </c>
+      <c r="K32" s="4">
         <f t="shared" ref="K32" si="21">GEOMEAN(K28:K31)</f>
-        <v>0.97200249761073332</v>
-      </c>
-      <c r="L32" s="3">
+        <v>0.96773607515230597</v>
+      </c>
+      <c r="L32" s="4">
         <f t="shared" ref="L32" si="22">GEOMEAN(L28:L31)</f>
-        <v>0.96752972409520555</v>
-      </c>
-      <c r="M32" s="3">
+        <v>0.97358047646493007</v>
+      </c>
+      <c r="M32" s="4">
         <f>GEOMEAN(M28:M31)</f>
-        <v>0.97020646010150124</v>
+        <v>0.96778385588480964</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -1532,7 +2610,7 @@
       <c r="L33" s="2"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A34" s="4"/>
+      <c r="A34" s="5"/>
       <c r="D34" s="1" t="s">
         <v>4</v>
       </c>
@@ -1545,7 +2623,7 @@
       <c r="L34" s="1"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A35" s="4"/>
+      <c r="A35" s="5"/>
       <c r="D35" s="2">
         <v>2</v>
       </c>
@@ -1572,7 +2650,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A36" s="4"/>
+      <c r="A36" s="5"/>
       <c r="B36" s="1" t="s">
         <v>5</v>
       </c>
@@ -1580,17 +2658,17 @@
         <v>0</v>
       </c>
       <c r="D36" s="3">
-        <v>1.0192495180162799</v>
+        <v>1.02841013900781</v>
       </c>
       <c r="E36" s="3">
-        <v>1.0026874087251001</v>
+        <v>1.0063014214122601</v>
       </c>
       <c r="F36" s="3">
-        <v>0.99301168657704497</v>
-      </c>
-      <c r="G36" s="3">
+        <v>1.02662132634825</v>
+      </c>
+      <c r="G36" s="4">
         <f>GEOMEAN(D36:F36)</f>
-        <v>1.0049246021525686</v>
+        <v>1.0203948057283321</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>5</v>
@@ -1599,95 +2677,95 @@
         <v>0</v>
       </c>
       <c r="J36" s="3">
-        <v>0.97089246137521901</v>
+        <v>0.95063087802887303</v>
       </c>
       <c r="K36" s="3">
-        <v>0.96600710193098804</v>
+        <v>0.95405184589922698</v>
       </c>
       <c r="L36" s="3">
-        <v>0.95466546425786303</v>
-      </c>
-      <c r="M36" s="3">
+        <v>0.96497369232735397</v>
+      </c>
+      <c r="M36" s="4">
         <f>GEOMEAN(J36:L36)</f>
-        <v>0.96383099153208351</v>
+        <v>0.95653262823580587</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A37" s="4"/>
+      <c r="A37" s="5"/>
       <c r="B37" s="1"/>
       <c r="C37" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D37" s="3">
-        <v>1.0251418452082599</v>
+        <v>1.0372909143167199</v>
       </c>
       <c r="E37" s="3">
-        <v>1.0046979309778701</v>
+        <v>1.0153450654570799</v>
       </c>
       <c r="F37" s="3">
-        <v>0.99258218072511795</v>
-      </c>
-      <c r="G37" s="3">
+        <v>1.0284804317546199</v>
+      </c>
+      <c r="G37" s="4">
         <f t="shared" ref="G37:G39" si="23">GEOMEAN(D37:F37)</f>
-        <v>1.0073846163226239</v>
+        <v>1.0269991634116376</v>
       </c>
       <c r="H37" s="1"/>
       <c r="I37" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J37" s="3">
-        <v>0.97734009021962798</v>
+        <v>0.963669704838515</v>
       </c>
       <c r="K37" s="3">
-        <v>0.976632558590939</v>
+        <v>0.96782692161109696</v>
       </c>
       <c r="L37" s="3">
-        <v>0.97793205868625099</v>
-      </c>
-      <c r="M37" s="3">
+        <v>0.97853919737083295</v>
+      </c>
+      <c r="M37" s="4">
         <f t="shared" ref="M37:M39" si="24">GEOMEAN(J37:L37)</f>
-        <v>0.97730142478686299</v>
+        <v>0.96999175747240807</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A38" s="4"/>
+      <c r="A38" s="5"/>
       <c r="B38" s="1"/>
       <c r="C38" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D38" s="3">
-        <v>1.0215852208309399</v>
+        <v>1.0328736856706799</v>
       </c>
       <c r="E38" s="3">
-        <v>0.99985821094038296</v>
+        <v>1.01342860315996</v>
       </c>
       <c r="F38" s="3">
-        <v>0.98860953121803297</v>
-      </c>
-      <c r="G38" s="3">
+        <v>1.0153457261427099</v>
+      </c>
+      <c r="G38" s="4">
         <f t="shared" si="23"/>
-        <v>1.0032579365103194</v>
+        <v>1.0205119752066012</v>
       </c>
       <c r="H38" s="1"/>
       <c r="I38" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J38" s="3">
-        <v>0.96820482438339195</v>
+        <v>0.95902719177627305</v>
       </c>
       <c r="K38" s="3">
-        <v>0.96649304441106498</v>
+        <v>0.96258651055766498</v>
       </c>
       <c r="L38" s="3">
-        <v>0.95792186849710503</v>
-      </c>
-      <c r="M38" s="3">
+        <v>0.96466391424303299</v>
+      </c>
+      <c r="M38" s="4">
         <f t="shared" si="24"/>
-        <v>0.96419606418015613</v>
+        <v>0.96208972200007081</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A39" s="4"/>
+      <c r="A39" s="5"/>
       <c r="B39" s="1"/>
       <c r="C39" s="2" t="s">
         <v>3</v>
@@ -1701,7 +2779,7 @@
       <c r="F39" s="3">
         <v>0.99082766719513404</v>
       </c>
-      <c r="G39" s="3">
+      <c r="G39" s="4">
         <f t="shared" si="23"/>
         <v>1.004875579795937</v>
       </c>
@@ -1718,7 +2796,7 @@
       <c r="L39" s="3">
         <v>0.94332758591741706</v>
       </c>
-      <c r="M39" s="3">
+      <c r="M39" s="4">
         <f t="shared" si="24"/>
         <v>0.94945936942928222</v>
       </c>
@@ -1727,44 +2805,44 @@
       <c r="C40" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="4">
         <f>GEOMEAN(D36:D39)</f>
-        <v>1.0216862581405359</v>
-      </c>
-      <c r="E40" s="3">
+        <v>1.0298199879930348</v>
+      </c>
+      <c r="E40" s="4">
         <f t="shared" ref="E40" si="25">GEOMEAN(E36:E39)</f>
-        <v>1.0026209542051379</v>
-      </c>
-      <c r="F40" s="3">
+        <v>1.009568128792443</v>
+      </c>
+      <c r="F40" s="4">
         <f t="shared" ref="F40" si="26">GEOMEAN(F36:F39)</f>
-        <v>0.99125624868288065</v>
-      </c>
-      <c r="G40" s="3">
+        <v>1.0152069827407264</v>
+      </c>
+      <c r="G40" s="4">
         <f>GEOMEAN(G36:G39)</f>
-        <v>1.0051096029948878</v>
+        <v>1.018162697334678</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J40" s="3">
+      <c r="J40" s="4">
         <f>GEOMEAN(J36:J39)</f>
-        <v>0.96738822970176896</v>
-      </c>
-      <c r="K40" s="3">
+        <v>0.9566378031095315</v>
+      </c>
+      <c r="K40" s="4">
         <f t="shared" ref="K40" si="27">GEOMEAN(K36:K39)</f>
-        <v>0.96519361363563094</v>
-      </c>
-      <c r="L40" s="3">
+        <v>0.95904555870735841</v>
+      </c>
+      <c r="L40" s="4">
         <f t="shared" ref="L40" si="28">GEOMEAN(L36:L39)</f>
-        <v>0.95838085506638482</v>
-      </c>
-      <c r="M40" s="3">
+        <v>0.96279331692144232</v>
+      </c>
+      <c r="M40" s="4">
         <f>GEOMEAN(M36:M39)</f>
-        <v>0.96364659102175099</v>
+        <v>0.9594888849411255</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -1783,7 +2861,7 @@
       <c r="L41" s="2"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A42" s="4"/>
+      <c r="A42" s="5"/>
       <c r="D42" s="1" t="s">
         <v>4</v>
       </c>
@@ -1796,7 +2874,7 @@
       <c r="L42" s="1"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A43" s="4"/>
+      <c r="A43" s="5"/>
       <c r="D43" s="2">
         <v>2</v>
       </c>
@@ -1823,7 +2901,7 @@
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A44" s="4"/>
+      <c r="A44" s="5"/>
       <c r="B44" s="1" t="s">
         <v>5</v>
       </c>
@@ -1831,17 +2909,17 @@
         <v>0</v>
       </c>
       <c r="D44" s="3">
-        <v>1.0186667995000001</v>
+        <v>1.0252949285986499</v>
       </c>
       <c r="E44" s="3">
-        <v>0.99744191792748205</v>
+        <v>1.0028969133834</v>
       </c>
       <c r="F44" s="3">
-        <v>0.98666124171407998</v>
-      </c>
-      <c r="G44" s="3">
+        <v>1.02192412461684</v>
+      </c>
+      <c r="G44" s="4">
         <f>GEOMEAN(D44:F44)</f>
-        <v>1.000835293620346</v>
+        <v>1.0166573042097149</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>5</v>
@@ -1850,95 +2928,95 @@
         <v>0</v>
       </c>
       <c r="J44" s="3">
-        <v>0.96988839282217498</v>
+        <v>0.94857968695696704</v>
       </c>
       <c r="K44" s="3">
-        <v>0.95934187762089596</v>
+        <v>0.94986019613639705</v>
       </c>
       <c r="L44" s="3">
-        <v>0.95280425191152696</v>
-      </c>
-      <c r="M44" s="3">
+        <v>0.96414048159349297</v>
+      </c>
+      <c r="M44" s="4">
         <f>GEOMEAN(J44:L44)</f>
-        <v>0.96065242586755495</v>
+        <v>0.95416747628198195</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A45" s="4"/>
+      <c r="A45" s="5"/>
       <c r="B45" s="1"/>
       <c r="C45" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D45" s="3">
-        <v>1.0263981275096099</v>
+        <v>1.0346255048737201</v>
       </c>
       <c r="E45" s="3">
-        <v>1.00264688798904</v>
+        <v>1.01239308989587</v>
       </c>
       <c r="F45" s="3">
-        <v>0.98987671919241005</v>
-      </c>
-      <c r="G45" s="3">
+        <v>1.0253365206937</v>
+      </c>
+      <c r="G45" s="4">
         <f t="shared" ref="G45:G47" si="29">GEOMEAN(D45:F45)</f>
-        <v>1.0061938468504497</v>
+        <v>1.0240777402949637</v>
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J45" s="3">
-        <v>0.97905062324657099</v>
+        <v>0.95813276472404296</v>
       </c>
       <c r="K45" s="3">
-        <v>0.97377485717950396</v>
+        <v>0.96198902394411301</v>
       </c>
       <c r="L45" s="3">
-        <v>0.97886517041826404</v>
-      </c>
-      <c r="M45" s="3">
+        <v>0.97686064041802501</v>
+      </c>
+      <c r="M45" s="4">
         <f t="shared" ref="M45:M47" si="30">GEOMEAN(J45:L45)</f>
-        <v>0.97722715598962417</v>
+        <v>0.96562716170079643</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A46" s="4"/>
+      <c r="A46" s="5"/>
       <c r="B46" s="1"/>
       <c r="C46" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D46" s="3">
-        <v>1.01963646017178</v>
+        <v>1.0307590369843</v>
       </c>
       <c r="E46" s="3">
-        <v>0.99761480192251595</v>
+        <v>1.0099022198748799</v>
       </c>
       <c r="F46" s="3">
-        <v>0.98610088991341804</v>
-      </c>
-      <c r="G46" s="3">
+        <v>1.0120933199253099</v>
+      </c>
+      <c r="G46" s="4">
         <f t="shared" si="29"/>
-        <v>1.0010210201497807</v>
+        <v>1.0175420029583118</v>
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J46" s="3">
-        <v>0.96469649160055804</v>
+        <v>0.95346949384957302</v>
       </c>
       <c r="K46" s="3">
-        <v>0.96031921584968005</v>
+        <v>0.95571689914513103</v>
       </c>
       <c r="L46" s="3">
-        <v>0.95669854312700797</v>
-      </c>
-      <c r="M46" s="3">
+        <v>0.96269405310159095</v>
+      </c>
+      <c r="M46" s="4">
         <f t="shared" si="30"/>
-        <v>0.96056585232494185</v>
+        <v>0.95728543729748417</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A47" s="4"/>
+      <c r="A47" s="5"/>
       <c r="B47" s="1"/>
       <c r="C47" s="2" t="s">
         <v>3</v>
@@ -1952,7 +3030,7 @@
       <c r="F47" s="3">
         <v>0.98950682924934996</v>
       </c>
-      <c r="G47" s="3">
+      <c r="G47" s="4">
         <f t="shared" si="29"/>
         <v>1.0009154789243422</v>
       </c>
@@ -1969,7 +3047,7 @@
       <c r="L47" s="3">
         <v>0.94167432746471103</v>
       </c>
-      <c r="M47" s="3">
+      <c r="M47" s="4">
         <f t="shared" si="30"/>
         <v>0.94424271972621476</v>
       </c>
@@ -1978,44 +3056,44 @@
       <c r="C48" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D48" s="4">
         <f>GEOMEAN(D44:D47)</f>
-        <v>1.0195185998530283</v>
-      </c>
-      <c r="E48" s="3">
+        <v>1.0259922932869916</v>
+      </c>
+      <c r="E48" s="4">
         <f t="shared" ref="E48" si="31">GEOMEAN(E44:E47)</f>
-        <v>0.99941570386574774</v>
-      </c>
-      <c r="F48" s="3">
+        <v>1.0062774490540221</v>
+      </c>
+      <c r="F48" s="4">
         <f t="shared" ref="F48" si="32">GEOMEAN(F44:F47)</f>
-        <v>0.98803500477309825</v>
-      </c>
-      <c r="G48" s="3">
+        <v>1.0121179055810423</v>
+      </c>
+      <c r="G48" s="4">
         <f>GEOMEAN(G44:G47)</f>
-        <v>1.0022388144534162</v>
+        <v>1.0147622801069813</v>
       </c>
       <c r="I48" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J48" s="3">
+      <c r="J48" s="4">
         <f>GEOMEAN(J44:J47)</f>
-        <v>0.96455706241903638</v>
-      </c>
-      <c r="K48" s="3">
+        <v>0.95126189751231793</v>
+      </c>
+      <c r="K48" s="4">
         <f t="shared" ref="K48" si="33">GEOMEAN(K44:K47)</f>
-        <v>0.95984459333487404</v>
-      </c>
-      <c r="L48" s="3">
+        <v>0.95340800928467118</v>
+      </c>
+      <c r="L48" s="4">
         <f t="shared" ref="L48" si="34">GEOMEAN(L44:L47)</f>
-        <v>0.95741582455526286</v>
-      </c>
-      <c r="M48" s="3">
+        <v>0.96125915108596383</v>
+      </c>
+      <c r="M48" s="4">
         <f>GEOMEAN(M44:M47)</f>
-        <v>0.96060125534867413</v>
+        <v>0.95530003781890815</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B49" s="2" t="s">
@@ -2034,7 +3112,7 @@
       <c r="L49" s="2"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A50" s="4"/>
+      <c r="A50" s="5"/>
       <c r="D50" s="1" t="s">
         <v>4</v>
       </c>
@@ -2047,7 +3125,7 @@
       <c r="L50" s="1"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A51" s="4"/>
+      <c r="A51" s="5"/>
       <c r="D51" s="2">
         <v>2</v>
       </c>
@@ -2074,7 +3152,7 @@
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A52" s="4"/>
+      <c r="A52" s="5"/>
       <c r="B52" s="1" t="s">
         <v>5</v>
       </c>
@@ -2082,17 +3160,17 @@
         <v>0</v>
       </c>
       <c r="D52" s="3">
-        <v>1.0560028666811001</v>
+        <v>1.0692381859906299</v>
       </c>
       <c r="E52" s="3">
-        <v>1.0300895307767399</v>
+        <v>1.0373160385958999</v>
       </c>
       <c r="F52" s="3">
-        <v>0.98635415695973006</v>
-      </c>
-      <c r="G52" s="3">
+        <v>1.0232560637229</v>
+      </c>
+      <c r="G52" s="4">
         <f>GEOMEAN(D52:F52)</f>
-        <v>1.023743089581012</v>
+        <v>1.0430936303680722</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>5</v>
@@ -2101,95 +3179,95 @@
         <v>0</v>
       </c>
       <c r="J52" s="3">
-        <v>0.98476580582929796</v>
+        <v>0.96812571259787406</v>
       </c>
       <c r="K52" s="3">
-        <v>0.97406781301402401</v>
+        <v>0.96707352322590001</v>
       </c>
       <c r="L52" s="3">
-        <v>0.94339941913073</v>
-      </c>
-      <c r="M52" s="3">
+        <v>0.96357050378850695</v>
+      </c>
+      <c r="M52" s="4">
         <f>GEOMEAN(J52:L52)</f>
-        <v>0.9672511449502833</v>
+        <v>0.96625461618062802</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A53" s="4"/>
+      <c r="A53" s="5"/>
       <c r="B53" s="1"/>
       <c r="C53" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D53" s="3">
-        <v>1.05240417738433</v>
+        <v>1.0711509833739401</v>
       </c>
       <c r="E53" s="3">
-        <v>1.0247149521065799</v>
+        <v>1.0357229311486</v>
       </c>
       <c r="F53" s="3">
-        <v>0.98791936967917304</v>
-      </c>
-      <c r="G53" s="3">
+        <v>1.02451298815799</v>
+      </c>
+      <c r="G53" s="4">
         <f t="shared" ref="G53:G55" si="35">GEOMEAN(D53:F53)</f>
-        <v>1.0213369536742078</v>
+        <v>1.0436076413229503</v>
       </c>
       <c r="H53" s="1"/>
       <c r="I53" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J53" s="3">
-        <v>0.981048284083607</v>
+        <v>0.97782040839761697</v>
       </c>
       <c r="K53" s="3">
-        <v>0.97722107243699396</v>
+        <v>0.97793251173983098</v>
       </c>
       <c r="L53" s="3">
-        <v>0.96213347984987097</v>
-      </c>
-      <c r="M53" s="3">
+        <v>0.98351939162804103</v>
+      </c>
+      <c r="M53" s="4">
         <f t="shared" ref="M53:M55" si="36">GEOMEAN(J53:L53)</f>
-        <v>0.97343325260570868</v>
+        <v>0.97975382961618729</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A54" s="4"/>
+      <c r="A54" s="5"/>
       <c r="B54" s="1"/>
       <c r="C54" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D54" s="3">
-        <v>1.0516967094938401</v>
+        <v>1.0665521648848599</v>
       </c>
       <c r="E54" s="3">
-        <v>1.02520003898663</v>
+        <v>1.0356716865346001</v>
       </c>
       <c r="F54" s="3">
-        <v>1.0020520981041301</v>
-      </c>
-      <c r="G54" s="3">
+        <v>1.0212169168872001</v>
+      </c>
+      <c r="G54" s="4">
         <f t="shared" si="35"/>
-        <v>1.0261160411788695</v>
+        <v>1.0409760439932174</v>
       </c>
       <c r="H54" s="1"/>
       <c r="I54" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J54" s="3">
-        <v>0.97818859894856203</v>
+        <v>0.97460928398468805</v>
       </c>
       <c r="K54" s="3">
-        <v>0.98147652920477502</v>
+        <v>0.98008723465191205</v>
       </c>
       <c r="L54" s="3">
-        <v>0.97346946386611299</v>
-      </c>
-      <c r="M54" s="3">
+        <v>0.977253918405941</v>
+      </c>
+      <c r="M54" s="4">
         <f t="shared" si="36"/>
-        <v>0.97770600523486706</v>
+        <v>0.97731425279212136</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A55" s="4"/>
+      <c r="A55" s="5"/>
       <c r="B55" s="1"/>
       <c r="C55" s="2" t="s">
         <v>3</v>
@@ -2203,7 +3281,7 @@
       <c r="F55" s="3">
         <v>0.98599374283393504</v>
       </c>
-      <c r="G55" s="3">
+      <c r="G55" s="4">
         <f t="shared" si="35"/>
         <v>1.0181954709349592</v>
       </c>
@@ -2220,7 +3298,7 @@
       <c r="L55" s="3">
         <v>0.96014742398462605</v>
       </c>
-      <c r="M55" s="3">
+      <c r="M55" s="4">
         <f t="shared" si="36"/>
         <v>0.96484718888082177</v>
       </c>
@@ -2229,44 +3307,44 @@
       <c r="C56" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D56" s="3">
+      <c r="D56" s="4">
         <f>GEOMEAN(D52:D55)</f>
-        <v>1.0507308520989349</v>
-      </c>
-      <c r="E56" s="3">
+        <v>1.062389460846165</v>
+      </c>
+      <c r="E56" s="4">
         <f t="shared" ref="E56" si="37">GEOMEAN(E52:E55)</f>
-        <v>1.0266432487694419</v>
-      </c>
-      <c r="F56" s="3">
+        <v>1.0338132342949369</v>
+      </c>
+      <c r="F56" s="4">
         <f t="shared" ref="F56" si="38">GEOMEAN(F52:F55)</f>
-        <v>0.99055754449080924</v>
-      </c>
-      <c r="G56" s="3">
+        <v>1.0136160732704935</v>
+      </c>
+      <c r="G56" s="4">
         <f>GEOMEAN(G52:G55)</f>
-        <v>1.0223436802707195</v>
+        <v>1.0364136160503963</v>
       </c>
       <c r="I56" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J56" s="3">
+      <c r="J56" s="4">
         <f>GEOMEAN(J52:J55)</f>
-        <v>0.9768795934161153</v>
-      </c>
-      <c r="K56" s="3">
+        <v>0.97103503977214545</v>
+      </c>
+      <c r="K56" s="4">
         <f t="shared" ref="K56" si="39">GEOMEAN(K52:K55)</f>
-        <v>0.97587760713324423</v>
-      </c>
-      <c r="L56" s="3">
+        <v>0.97395332955890113</v>
+      </c>
+      <c r="L56" s="4">
         <f t="shared" ref="L56" si="40">GEOMEAN(L52:L55)</f>
-        <v>0.95972718446173111</v>
-      </c>
-      <c r="M56" s="3">
+        <v>0.97107537555769785</v>
+      </c>
+      <c r="M56" s="4">
         <f>GEOMEAN(M52:M55)</f>
-        <v>0.97079618767744014</v>
+        <v>0.97202028869485435</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B57" s="2" t="s">
@@ -2285,7 +3363,7 @@
       <c r="L57" s="2"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A58" s="4"/>
+      <c r="A58" s="5"/>
       <c r="D58" s="1" t="s">
         <v>4</v>
       </c>
@@ -2298,7 +3376,7 @@
       <c r="L58" s="1"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A59" s="4"/>
+      <c r="A59" s="5"/>
       <c r="D59" s="2">
         <v>2</v>
       </c>
@@ -2325,7 +3403,7 @@
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A60" s="4"/>
+      <c r="A60" s="5"/>
       <c r="B60" s="1" t="s">
         <v>5</v>
       </c>
@@ -2333,17 +3411,17 @@
         <v>0</v>
       </c>
       <c r="D60" s="3">
-        <v>1.0560028666811001</v>
+        <v>1.0692381859906299</v>
       </c>
       <c r="E60" s="3">
-        <v>1.04514005041323</v>
+        <v>1.0446037868689699</v>
       </c>
       <c r="F60" s="3">
-        <v>1.0614353954587701</v>
-      </c>
-      <c r="G60" s="3">
+        <v>1.06464481985759</v>
+      </c>
+      <c r="G60" s="4">
         <f>GEOMEAN(D60:F60)</f>
-        <v>1.0541709671513604</v>
+        <v>1.0594413852308702</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>5</v>
@@ -2352,95 +3430,95 @@
         <v>0</v>
       </c>
       <c r="J60" s="3">
-        <v>0.98476580582929796</v>
+        <v>0.96812571259787406</v>
       </c>
       <c r="K60" s="3">
-        <v>0.96975921926139896</v>
+        <v>0.96004000335051898</v>
       </c>
       <c r="L60" s="3">
-        <v>0.96692278063616599</v>
-      </c>
-      <c r="M60" s="3">
+        <v>0.96951317244848101</v>
+      </c>
+      <c r="M60" s="4">
         <f>GEOMEAN(J60:L60)</f>
-        <v>0.97378457249963346</v>
+        <v>0.96588391302539334</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A61" s="4"/>
+      <c r="A61" s="5"/>
       <c r="B61" s="1"/>
       <c r="C61" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D61" s="3">
-        <v>1.05240417738433</v>
+        <v>1.0711509833739401</v>
       </c>
       <c r="E61" s="3">
-        <v>1.02989623382075</v>
+        <v>1.0426158574501001</v>
       </c>
       <c r="F61" s="3">
-        <v>1.02556572594388</v>
-      </c>
-      <c r="G61" s="3">
+        <v>1.05090206061106</v>
+      </c>
+      <c r="G61" s="4">
         <f t="shared" ref="G61:G63" si="41">GEOMEAN(D61:F61)</f>
-        <v>1.0358888947648233</v>
+        <v>1.0548217757614406</v>
       </c>
       <c r="H61" s="1"/>
       <c r="I61" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J61" s="3">
-        <v>0.981048284083607</v>
+        <v>0.97782040839761697</v>
       </c>
       <c r="K61" s="3">
-        <v>0.96784352809116403</v>
+        <v>0.973761303851023</v>
       </c>
       <c r="L61" s="3">
-        <v>0.96393142703819201</v>
-      </c>
-      <c r="M61" s="3">
+        <v>0.98536255495520897</v>
+      </c>
+      <c r="M61" s="4">
         <f t="shared" ref="M61:M63" si="42">GEOMEAN(J61:L61)</f>
-        <v>0.97091353976565375</v>
+        <v>0.97896963493389888</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A62" s="4"/>
+      <c r="A62" s="5"/>
       <c r="B62" s="1"/>
       <c r="C62" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D62" s="3">
-        <v>1.0516967094938401</v>
+        <v>1.0665521648848599</v>
       </c>
       <c r="E62" s="3">
-        <v>1.0302068435918801</v>
+        <v>1.03834990632317</v>
       </c>
       <c r="F62" s="3">
-        <v>1.0291684809974999</v>
-      </c>
-      <c r="G62" s="3">
+        <v>1.04067227862718</v>
+      </c>
+      <c r="G62" s="4">
         <f t="shared" si="41"/>
-        <v>1.0369722652339226</v>
+        <v>1.0484472990085429</v>
       </c>
       <c r="H62" s="1"/>
       <c r="I62" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J62" s="3">
-        <v>0.97818859894856203</v>
+        <v>0.97460928398468805</v>
       </c>
       <c r="K62" s="3">
-        <v>0.97773742911510697</v>
+        <v>0.97395690018127301</v>
       </c>
       <c r="L62" s="3">
-        <v>0.97495046668101903</v>
-      </c>
-      <c r="M62" s="3">
+        <v>0.981666882042458</v>
+      </c>
+      <c r="M62" s="4">
         <f t="shared" si="42"/>
-        <v>0.97695778138125589</v>
+        <v>0.97673812723768083</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A63" s="4"/>
+      <c r="A63" s="5"/>
       <c r="B63" s="1"/>
       <c r="C63" s="2" t="s">
         <v>3</v>
@@ -2454,7 +3532,7 @@
       <c r="F63" s="3">
         <v>1.0053536802576299</v>
       </c>
-      <c r="G63" s="3">
+      <c r="G63" s="4">
         <f t="shared" si="41"/>
         <v>1.0226343012112742</v>
       </c>
@@ -2471,7 +3549,7 @@
       <c r="L63" s="3">
         <v>0.95960179803427204</v>
       </c>
-      <c r="M63" s="3">
+      <c r="M63" s="4">
         <f t="shared" si="42"/>
         <v>0.96250805467614375</v>
       </c>
@@ -2480,44 +3558,44 @@
       <c r="C64" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D64" s="3">
+      <c r="D64" s="4">
         <f>GEOMEAN(D60:D63)</f>
-        <v>1.0507308520989349</v>
-      </c>
-      <c r="E64" s="3">
+        <v>1.062389460846165</v>
+      </c>
+      <c r="E64" s="4">
         <f t="shared" ref="E64" si="43">GEOMEAN(E60:E63)</f>
-        <v>1.0312802626894364</v>
-      </c>
-      <c r="F64" s="3">
+        <v>1.0363549372319911</v>
+      </c>
+      <c r="F64" s="4">
         <f t="shared" ref="F64" si="44">GEOMEAN(F60:F63)</f>
-        <v>1.0301859045634911</v>
-      </c>
-      <c r="G64" s="3">
+        <v>1.0401595522577256</v>
+      </c>
+      <c r="G64" s="4">
         <f>GEOMEAN(G60:G63)</f>
-        <v>1.0373562581036178</v>
+        <v>1.0462386157374075</v>
       </c>
       <c r="I64" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J64" s="3">
+      <c r="J64" s="4">
         <f>GEOMEAN(J60:J63)</f>
-        <v>0.9768795934161153</v>
-      </c>
-      <c r="K64" s="3">
+        <v>0.97103503977214545</v>
+      </c>
+      <c r="K64" s="4">
         <f t="shared" ref="K64" si="45">GEOMEAN(K60:K63)</f>
-        <v>0.96989292327757304</v>
-      </c>
-      <c r="L64" s="3">
+        <v>0.96799108751991758</v>
+      </c>
+      <c r="L64" s="4">
         <f t="shared" ref="L64" si="46">GEOMEAN(L60:L63)</f>
-        <v>0.96633538824064924</v>
-      </c>
-      <c r="M64" s="3">
+        <v>0.97398269410359695</v>
+      </c>
+      <c r="M64" s="4">
         <f>GEOMEAN(M60:M63)</f>
-        <v>0.97102610155110758</v>
+        <v>0.970999859137338</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A65" s="4" t="s">
+      <c r="A65" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B65" s="2" t="s">
@@ -2536,7 +3614,7 @@
       <c r="L65" s="2"/>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A66" s="4"/>
+      <c r="A66" s="5"/>
       <c r="D66" s="1" t="s">
         <v>4</v>
       </c>
@@ -2549,7 +3627,7 @@
       <c r="L66" s="1"/>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A67" s="4"/>
+      <c r="A67" s="5"/>
       <c r="D67" s="2">
         <v>2</v>
       </c>
@@ -2576,7 +3654,7 @@
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A68" s="4"/>
+      <c r="A68" s="5"/>
       <c r="B68" s="1" t="s">
         <v>5</v>
       </c>
@@ -2584,17 +3662,17 @@
         <v>0</v>
       </c>
       <c r="D68" s="3">
-        <v>1.03664691254328</v>
+        <v>1.05528639170465</v>
       </c>
       <c r="E68" s="3">
-        <v>1.0192976980091299</v>
+        <v>1.0273873034579499</v>
       </c>
       <c r="F68" s="3">
-        <v>0.98635415695973006</v>
-      </c>
-      <c r="G68" s="3">
+        <v>1.0232560637229</v>
+      </c>
+      <c r="G68" s="4">
         <f>GEOMEAN(D68:F68)</f>
-        <v>1.0138839786342964</v>
+        <v>1.0352127677125957</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>5</v>
@@ -2603,95 +3681,95 @@
         <v>0</v>
       </c>
       <c r="J68" s="3">
-        <v>0.97789174684545399</v>
+        <v>0.97384506446603503</v>
       </c>
       <c r="K68" s="3">
-        <v>0.96873836282442605</v>
+        <v>0.96859926003090802</v>
       </c>
       <c r="L68" s="3">
-        <v>0.94339941913073</v>
-      </c>
-      <c r="M68" s="3">
+        <v>0.96357050378850695</v>
+      </c>
+      <c r="M68" s="4">
         <f>GEOMEAN(J68:L68)</f>
-        <v>0.96323213131653851</v>
+        <v>0.96866252693817845</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A69" s="4"/>
+      <c r="A69" s="5"/>
       <c r="B69" s="1"/>
       <c r="C69" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D69" s="3">
-        <v>1.0408783191789901</v>
+        <v>1.06051822386519</v>
       </c>
       <c r="E69" s="3">
-        <v>1.0167662141720799</v>
+        <v>1.0290406582837901</v>
       </c>
       <c r="F69" s="3">
-        <v>0.98791936967917304</v>
-      </c>
-      <c r="G69" s="3">
+        <v>1.02451298815799</v>
+      </c>
+      <c r="G69" s="4">
         <f t="shared" ref="G69:G71" si="47">GEOMEAN(D69:F69)</f>
-        <v>1.0149567197863214</v>
+        <v>1.0379012768933922</v>
       </c>
       <c r="H69" s="1"/>
       <c r="I69" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J69" s="3">
-        <v>0.99132987974804798</v>
+        <v>0.98870407973306995</v>
       </c>
       <c r="K69" s="3">
-        <v>0.97699408982397695</v>
+        <v>0.98229246896209699</v>
       </c>
       <c r="L69" s="3">
-        <v>0.96213347984987097</v>
-      </c>
-      <c r="M69" s="3">
+        <v>0.98351939162804103</v>
+      </c>
+      <c r="M69" s="4">
         <f t="shared" ref="M69:M71" si="48">GEOMEAN(J69:L69)</f>
-        <v>0.97674640197213913</v>
+        <v>0.98483473094659624</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A70" s="4"/>
+      <c r="A70" s="5"/>
       <c r="B70" s="1"/>
       <c r="C70" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D70" s="3">
-        <v>1.04404619905733</v>
+        <v>1.0561804240519901</v>
       </c>
       <c r="E70" s="3">
-        <v>1.02476962005954</v>
+        <v>1.0329765565644999</v>
       </c>
       <c r="F70" s="3">
-        <v>1.0020520981041301</v>
-      </c>
-      <c r="G70" s="3">
+        <v>1.0212169168872001</v>
+      </c>
+      <c r="G70" s="4">
         <f t="shared" si="47"/>
-        <v>1.0234785694756992</v>
+        <v>1.0366898818797889</v>
       </c>
       <c r="H70" s="1"/>
       <c r="I70" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J70" s="3">
-        <v>0.98812604975715801</v>
+        <v>0.980326215102578</v>
       </c>
       <c r="K70" s="3">
-        <v>0.98732450172187503</v>
+        <v>0.98309358377894696</v>
       </c>
       <c r="L70" s="3">
-        <v>0.97346946386611299</v>
-      </c>
-      <c r="M70" s="3">
+        <v>0.977253918405941</v>
+      </c>
+      <c r="M70" s="4">
         <f t="shared" si="48"/>
-        <v>0.9829502378844821</v>
+        <v>0.98022167034575891</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A71" s="4"/>
+      <c r="A71" s="5"/>
       <c r="B71" s="1"/>
       <c r="C71" s="2" t="s">
         <v>3</v>
@@ -2705,7 +3783,7 @@
       <c r="F71" s="3">
         <v>0.98599374283393504</v>
       </c>
-      <c r="G71" s="3">
+      <c r="G71" s="4">
         <f t="shared" si="47"/>
         <v>1.0155983824502794</v>
       </c>
@@ -2722,7 +3800,7 @@
       <c r="L71" s="3">
         <v>0.96014742398462605</v>
       </c>
-      <c r="M71" s="3">
+      <c r="M71" s="4">
         <f t="shared" si="48"/>
         <v>0.96829327509781937</v>
       </c>
@@ -2731,44 +3809,44 @@
       <c r="C72" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D72" s="3">
+      <c r="D72" s="4">
         <f>GEOMEAN(D68:D71)</f>
-        <v>1.0398699820774133</v>
-      </c>
-      <c r="E72" s="3">
+        <v>1.0524417159171073</v>
+      </c>
+      <c r="E72" s="4">
         <f t="shared" ref="E72" si="49">GEOMEAN(E68:E71)</f>
-        <v>1.0211008824376966</v>
-      </c>
-      <c r="F72" s="3">
+        <v>1.0282432139784359</v>
+      </c>
+      <c r="F72" s="4">
         <f t="shared" ref="F72" si="50">GEOMEAN(F68:F71)</f>
-        <v>0.99055754449080924</v>
-      </c>
-      <c r="G72" s="3">
+        <v>1.0136160732704935</v>
+      </c>
+      <c r="G72" s="4">
         <f>GEOMEAN(G68:G71)</f>
-        <v>1.0169723246074449</v>
+        <v>1.0313097689495503</v>
       </c>
       <c r="I72" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J72" s="3">
+      <c r="J72" s="4">
         <f>GEOMEAN(J68:J71)</f>
-        <v>0.98177459825749458</v>
-      </c>
-      <c r="K72" s="3">
+        <v>0.97816734955117812</v>
+      </c>
+      <c r="K72" s="4">
         <f t="shared" ref="K72" si="51">GEOMEAN(K68:K71)</f>
-        <v>0.97696461489944353</v>
-      </c>
-      <c r="L72" s="3">
+        <v>0.97720166645794992</v>
+      </c>
+      <c r="L72" s="4">
         <f t="shared" ref="L72" si="52">GEOMEAN(L68:L71)</f>
-        <v>0.95972718446173111</v>
-      </c>
-      <c r="M72" s="3">
+        <v>0.97107537555769785</v>
+      </c>
+      <c r="M72" s="4">
         <f>GEOMEAN(M68:M71)</f>
-        <v>0.97277591037222833</v>
+        <v>0.97547640164003047</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A73" s="4" t="s">
+      <c r="A73" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B73" s="2" t="s">
@@ -2787,7 +3865,7 @@
       <c r="L73" s="2"/>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A74" s="4"/>
+      <c r="A74" s="5"/>
       <c r="D74" s="1" t="s">
         <v>4</v>
       </c>
@@ -2800,7 +3878,7 @@
       <c r="L74" s="1"/>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A75" s="4"/>
+      <c r="A75" s="5"/>
       <c r="D75" s="2">
         <v>2</v>
       </c>
@@ -2827,7 +3905,7 @@
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A76" s="4"/>
+      <c r="A76" s="5"/>
       <c r="B76" s="1" t="s">
         <v>5</v>
       </c>
@@ -2835,17 +3913,17 @@
         <v>0</v>
       </c>
       <c r="D76" s="3">
-        <v>1.0430888595391199</v>
+        <v>1.06491700073463</v>
       </c>
       <c r="E76" s="3">
-        <v>1.0300895307767399</v>
+        <v>1.0373160385958999</v>
       </c>
       <c r="F76" s="3">
-        <v>1.0104317267674401</v>
-      </c>
-      <c r="G76" s="3">
+        <v>1.04333198348207</v>
+      </c>
+      <c r="G76" s="4">
         <f>GEOMEAN(D76:F76)</f>
-        <v>1.0277821832698124</v>
+        <v>1.0484549908751406</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>5</v>
@@ -2854,95 +3932,95 @@
         <v>0</v>
       </c>
       <c r="J76" s="3">
-        <v>0.983410553496049</v>
+        <v>0.97499139368472798</v>
       </c>
       <c r="K76" s="3">
-        <v>0.97406781301402401</v>
+        <v>0.96707352322590001</v>
       </c>
       <c r="L76" s="3">
-        <v>0.95246069446966497</v>
-      </c>
-      <c r="M76" s="3">
+        <v>0.961827657332185</v>
+      </c>
+      <c r="M76" s="4">
         <f>GEOMEAN(J76:L76)</f>
-        <v>0.96989273589663927</v>
+        <v>0.96794908170869476</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A77" s="4"/>
+      <c r="A77" s="5"/>
       <c r="B77" s="1"/>
       <c r="C77" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D77" s="3">
-        <v>1.04589796390991</v>
+        <v>1.07170009126761</v>
       </c>
       <c r="E77" s="3">
-        <v>1.0247149521065799</v>
+        <v>1.0357229311486</v>
       </c>
       <c r="F77" s="3">
-        <v>0.99927086606341897</v>
-      </c>
-      <c r="G77" s="3">
+        <v>1.03106696316139</v>
+      </c>
+      <c r="G77" s="4">
         <f t="shared" ref="G77:G79" si="53">GEOMEAN(D77:F77)</f>
-        <v>1.0231167751776706</v>
+        <v>1.046006966630131</v>
       </c>
       <c r="H77" s="1"/>
       <c r="I77" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J77" s="3">
-        <v>0.98967053627197499</v>
+        <v>0.988581174720222</v>
       </c>
       <c r="K77" s="3">
-        <v>0.97722107243699396</v>
+        <v>0.97793251173983098</v>
       </c>
       <c r="L77" s="3">
-        <v>0.96176795584025399</v>
-      </c>
-      <c r="M77" s="3">
+        <v>0.97638156958579903</v>
+      </c>
+      <c r="M77" s="4">
         <f t="shared" ref="M77:M79" si="54">GEOMEAN(J77:L77)</f>
-        <v>0.97615306556628101</v>
+        <v>0.98095013485992444</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A78" s="4"/>
+      <c r="A78" s="5"/>
       <c r="B78" s="1"/>
       <c r="C78" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D78" s="3">
-        <v>1.05178407102322</v>
+        <v>1.0645365735836401</v>
       </c>
       <c r="E78" s="3">
-        <v>1.02520003898663</v>
+        <v>1.0356716865346001</v>
       </c>
       <c r="F78" s="3">
-        <v>1.0038753457952601</v>
-      </c>
-      <c r="G78" s="3">
+        <v>1.0240060676662399</v>
+      </c>
+      <c r="G78" s="4">
         <f t="shared" si="53"/>
-        <v>1.0267664368677509</v>
+        <v>1.0412661254658415</v>
       </c>
       <c r="H78" s="1"/>
       <c r="I78" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J78" s="3">
-        <v>0.98508629992611696</v>
+        <v>0.98212471393134704</v>
       </c>
       <c r="K78" s="3">
-        <v>0.98147652920477502</v>
+        <v>0.98008723465191205</v>
       </c>
       <c r="L78" s="3">
-        <v>0.96580136283538398</v>
-      </c>
-      <c r="M78" s="3">
+        <v>0.97495809057888005</v>
+      </c>
+      <c r="M78" s="4">
         <f t="shared" si="54"/>
-        <v>0.97741876031056163</v>
+        <v>0.97905203240516314</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A79" s="4"/>
+      <c r="A79" s="5"/>
       <c r="B79" s="1"/>
       <c r="C79" s="2" t="s">
         <v>3</v>
@@ -2956,7 +4034,7 @@
       <c r="F79" s="3">
         <v>0.99409806530988698</v>
       </c>
-      <c r="G79" s="3">
+      <c r="G79" s="4">
         <f t="shared" si="53"/>
         <v>1.0220754601760698</v>
       </c>
@@ -2973,7 +4051,7 @@
       <c r="L79" s="3">
         <v>0.95436363606061603</v>
       </c>
-      <c r="M79" s="3">
+      <c r="M79" s="4">
         <f t="shared" si="54"/>
         <v>0.96542039053213613</v>
       </c>
@@ -2982,44 +4060,44 @@
       <c r="C80" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D80" s="3">
+      <c r="D80" s="4">
         <f>GEOMEAN(D76:D79)</f>
-        <v>1.0467460403438213</v>
-      </c>
-      <c r="E80" s="3">
+        <v>1.0618041708519976</v>
+      </c>
+      <c r="E80" s="4">
         <f t="shared" ref="E80" si="55">GEOMEAN(E76:E79)</f>
-        <v>1.0266432487694419</v>
-      </c>
-      <c r="F80" s="3">
+        <v>1.0338132342949369</v>
+      </c>
+      <c r="F80" s="4">
         <f t="shared" ref="F80" si="56">GEOMEAN(F76:F79)</f>
-        <v>1.0019009865710609</v>
-      </c>
-      <c r="G80" s="3">
+        <v>1.0229638526728693</v>
+      </c>
+      <c r="G80" s="4">
         <f>GEOMEAN(G76:G79)</f>
-        <v>1.0249324156855644</v>
+        <v>1.0393989347860288</v>
       </c>
       <c r="I80" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J80" s="3">
+      <c r="J80" s="4">
         <f>GEOMEAN(J76:J79)</f>
-        <v>0.98232219520887121</v>
-      </c>
-      <c r="K80" s="3">
+        <v>0.97920573901728636</v>
+      </c>
+      <c r="K80" s="4">
         <f t="shared" ref="K80" si="57">GEOMEAN(K76:K79)</f>
-        <v>0.97587760713324423</v>
-      </c>
-      <c r="L80" s="3">
+        <v>0.97395332955890113</v>
+      </c>
+      <c r="L80" s="4">
         <f t="shared" ref="L80" si="58">GEOMEAN(L76:L79)</f>
-        <v>0.95858309481936532</v>
-      </c>
-      <c r="M80" s="3">
+        <v>0.96683901264654515</v>
+      </c>
+      <c r="M80" s="4">
         <f>GEOMEAN(M76:M79)</f>
-        <v>0.97220912221006583</v>
+        <v>0.97331949246072047</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A81" s="4" t="s">
+      <c r="A81" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B81" s="2" t="s">
@@ -3038,7 +4116,7 @@
       <c r="L81" s="2"/>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A82" s="4"/>
+      <c r="A82" s="5"/>
       <c r="D82" s="1" t="s">
         <v>4</v>
       </c>
@@ -3051,7 +4129,7 @@
       <c r="L82" s="1"/>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A83" s="4"/>
+      <c r="A83" s="5"/>
       <c r="D83" s="2">
         <v>2</v>
       </c>
@@ -3078,7 +4156,7 @@
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A84" s="4"/>
+      <c r="A84" s="5"/>
       <c r="B84" s="1" t="s">
         <v>5</v>
       </c>
@@ -3086,17 +4164,17 @@
         <v>0</v>
       </c>
       <c r="D84" s="3">
-        <v>1.02875980115403</v>
+        <v>1.04918905115572</v>
       </c>
       <c r="E84" s="3">
-        <v>1.0143215125323399</v>
+        <v>1.0243397169178201</v>
       </c>
       <c r="F84" s="3">
-        <v>0.982610540143668</v>
-      </c>
-      <c r="G84" s="3">
+        <v>1.0204885683275</v>
+      </c>
+      <c r="G84" s="4">
         <f>GEOMEAN(D84:F84)</f>
-        <v>1.0083787388208549</v>
+        <v>1.0312610980662456</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>5</v>
@@ -3105,95 +4183,95 @@
         <v>0</v>
       </c>
       <c r="J84" s="3">
-        <v>0.973670248568</v>
+        <v>0.96617793509254701</v>
       </c>
       <c r="K84" s="3">
-        <v>0.96469060805578299</v>
+        <v>0.96374765394973705</v>
       </c>
       <c r="L84" s="3">
-        <v>0.93899425652861901</v>
-      </c>
-      <c r="M84" s="3">
+        <v>0.95704960870377398</v>
+      </c>
+      <c r="M84" s="4">
         <f>GEOMEAN(J84:L84)</f>
-        <v>0.95900520001985667</v>
+        <v>0.96231731398504938</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A85" s="4"/>
+      <c r="A85" s="5"/>
       <c r="B85" s="1"/>
       <c r="C85" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D85" s="3">
-        <v>1.0344464226713199</v>
+        <v>1.05720963871041</v>
       </c>
       <c r="E85" s="3">
-        <v>1.0129024797652</v>
+        <v>1.02780806251239</v>
       </c>
       <c r="F85" s="3">
-        <v>0.98245128935401205</v>
-      </c>
-      <c r="G85" s="3">
+        <v>1.0187134313730399</v>
+      </c>
+      <c r="G85" s="4">
         <f t="shared" ref="G85:G87" si="59">GEOMEAN(D85:F85)</f>
-        <v>1.009707435586467</v>
+        <v>1.034447343782698</v>
       </c>
       <c r="H85" s="1"/>
       <c r="I85" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J85" s="3">
-        <v>0.98427514213697698</v>
+        <v>0.981766283622868</v>
       </c>
       <c r="K85" s="3">
-        <v>0.97357052193928895</v>
+        <v>0.97808571687003298</v>
       </c>
       <c r="L85" s="3">
-        <v>0.95695209015229699</v>
-      </c>
-      <c r="M85" s="3">
+        <v>0.97667969475628102</v>
+      </c>
+      <c r="M85" s="4">
         <f t="shared" ref="M85:M87" si="60">GEOMEAN(J85:L85)</f>
-        <v>0.97153408697136534</v>
+        <v>0.97884155054672783</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A86" s="4"/>
+      <c r="A86" s="5"/>
       <c r="B86" s="1"/>
       <c r="C86" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D86" s="3">
-        <v>1.0408545472886599</v>
+        <v>1.05377881022233</v>
       </c>
       <c r="E86" s="3">
-        <v>1.0226634094515901</v>
+        <v>1.0319375803820701</v>
       </c>
       <c r="F86" s="3">
-        <v>0.99648497501194</v>
-      </c>
-      <c r="G86" s="3">
+        <v>1.0158663467400899</v>
+      </c>
+      <c r="G86" s="4">
         <f t="shared" si="59"/>
-        <v>1.0198379575042755</v>
+        <v>1.0337443632101575</v>
       </c>
       <c r="H86" s="1"/>
       <c r="I86" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J86" s="3">
-        <v>0.98139705958864498</v>
+        <v>0.97454052166222505</v>
       </c>
       <c r="K86" s="3">
-        <v>0.98371678418429298</v>
+        <v>0.97903950113632299</v>
       </c>
       <c r="L86" s="3">
-        <v>0.96706198860893799</v>
-      </c>
-      <c r="M86" s="3">
+        <v>0.97252524142185204</v>
+      </c>
+      <c r="M86" s="4">
         <f t="shared" si="60"/>
-        <v>0.97736409916666156</v>
+        <v>0.97536462313530448</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A87" s="4"/>
+      <c r="A87" s="5"/>
       <c r="B87" s="1"/>
       <c r="C87" s="2" t="s">
         <v>3</v>
@@ -3207,7 +4285,7 @@
       <c r="F87" s="3">
         <v>0.983536624131786</v>
       </c>
-      <c r="G87" s="3">
+      <c r="G87" s="4">
         <f t="shared" si="59"/>
         <v>1.0122263025573053</v>
       </c>
@@ -3224,7 +4302,7 @@
       <c r="L87" s="3">
         <v>0.95529480361190999</v>
       </c>
-      <c r="M87" s="3">
+      <c r="M87" s="4">
         <f t="shared" si="60"/>
         <v>0.96347062126196248</v>
       </c>
@@ -3233,44 +4311,44 @@
       <c r="C88" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D88" s="3">
+      <c r="D88" s="4">
         <f>GEOMEAN(D84:D87)</f>
-        <v>1.0342841725140952</v>
-      </c>
-      <c r="E88" s="3">
+        <v>1.0482815740655447</v>
+      </c>
+      <c r="E88" s="4">
         <f t="shared" ref="E88" si="61">GEOMEAN(E84:E87)</f>
-        <v>1.0176365705583177</v>
-      </c>
-      <c r="F88" s="3">
+        <v>1.0261859727870968</v>
+      </c>
+      <c r="F88" s="4">
         <f t="shared" ref="F88" si="62">GEOMEAN(F84:F87)</f>
-        <v>0.98625322000255589</v>
-      </c>
-      <c r="G88" s="3">
+        <v>1.0095360257041519</v>
+      </c>
+      <c r="G88" s="4">
         <f>GEOMEAN(G84:G87)</f>
-        <v>1.0125279169526671</v>
+        <v>1.027878895513928</v>
       </c>
       <c r="I88" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J88" s="3">
+      <c r="J88" s="4">
         <f>GEOMEAN(J84:J87)</f>
-        <v>0.97576568890492577</v>
-      </c>
-      <c r="K88" s="3">
+        <v>0.97155755447212189</v>
+      </c>
+      <c r="K88" s="4">
         <f t="shared" ref="K88" si="63">GEOMEAN(K84:K87)</f>
-        <v>0.97330429509745442</v>
-      </c>
-      <c r="L88" s="3">
+        <v>0.97303255168101355</v>
+      </c>
+      <c r="L88" s="4">
         <f t="shared" ref="L88" si="64">GEOMEAN(L84:L87)</f>
-        <v>0.95452259871679979</v>
-      </c>
-      <c r="M88" s="3">
+        <v>0.96534205495463998</v>
+      </c>
+      <c r="M88" s="4">
         <f>GEOMEAN(M84:M87)</f>
-        <v>0.96781748923128885</v>
+        <v>0.96997165432465027</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A89" s="4" t="s">
+      <c r="A89" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B89" s="2" t="s">
@@ -3289,7 +4367,7 @@
       <c r="L89" s="2"/>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A90" s="4"/>
+      <c r="A90" s="5"/>
       <c r="D90" s="1" t="s">
         <v>4</v>
       </c>
@@ -3302,7 +4380,7 @@
       <c r="L90" s="1"/>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A91" s="4"/>
+      <c r="A91" s="5"/>
       <c r="D91" s="2">
         <v>2</v>
       </c>
@@ -3329,7 +4407,7 @@
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A92" s="4"/>
+      <c r="A92" s="5"/>
       <c r="B92" s="1" t="s">
         <v>5</v>
       </c>
@@ -3337,17 +4415,17 @@
         <v>0</v>
       </c>
       <c r="D92" s="3">
-        <v>1.02452427600744</v>
+        <v>1.04191466518083</v>
       </c>
       <c r="E92" s="3">
-        <v>0.99908625279937402</v>
+        <v>1.0185874630300999</v>
       </c>
       <c r="F92" s="3">
-        <v>0.98244475038630896</v>
-      </c>
-      <c r="G92" s="3">
+        <v>1.0281353455919899</v>
+      </c>
+      <c r="G92" s="4">
         <f>GEOMEAN(D92:F92)</f>
-        <v>1.0018694280188962</v>
+        <v>1.0295013545331364</v>
       </c>
       <c r="H92" s="1" t="s">
         <v>5</v>
@@ -3356,95 +4434,95 @@
         <v>0</v>
       </c>
       <c r="J92" s="3">
-        <v>0.97236635060482701</v>
+        <v>0.96235863850553605</v>
       </c>
       <c r="K92" s="3">
-        <v>0.95184420740491604</v>
+        <v>0.95388587731580099</v>
       </c>
       <c r="L92" s="3">
-        <v>0.93723991258994799</v>
-      </c>
-      <c r="M92" s="3">
+        <v>0.96009149863014198</v>
+      </c>
+      <c r="M92" s="4">
         <f>GEOMEAN(J92:L92)</f>
-        <v>0.95370821269877637</v>
+        <v>0.95877197418714699</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A93" s="4"/>
+      <c r="A93" s="5"/>
       <c r="B93" s="1"/>
       <c r="C93" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D93" s="3">
-        <v>1.03069157498098</v>
+        <v>1.04715659414977</v>
       </c>
       <c r="E93" s="3">
-        <v>1.0049987069081401</v>
+        <v>1.0191612029375801</v>
       </c>
       <c r="F93" s="3">
-        <v>0.98492474016827103</v>
-      </c>
-      <c r="G93" s="3">
+        <v>1.0174152882174401</v>
+      </c>
+      <c r="G93" s="4">
         <f t="shared" ref="G93:G95" si="65">GEOMEAN(D93:F93)</f>
-        <v>1.0066977358988565</v>
+        <v>1.0278212474339543</v>
       </c>
       <c r="H93" s="1"/>
       <c r="I93" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J93" s="3">
-        <v>0.98339897773952401</v>
+        <v>0.97328510956004799</v>
       </c>
       <c r="K93" s="3">
-        <v>0.96787464352839903</v>
+        <v>0.96817232647983997</v>
       </c>
       <c r="L93" s="3">
-        <v>0.96343768667947305</v>
-      </c>
-      <c r="M93" s="3">
+        <v>0.97674527765150998</v>
+      </c>
+      <c r="M93" s="4">
         <f t="shared" ref="M93:M95" si="66">GEOMEAN(J93:L93)</f>
-        <v>0.97153286939851835</v>
+        <v>0.97272786001530254</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A94" s="4"/>
+      <c r="A94" s="5"/>
       <c r="B94" s="1"/>
       <c r="C94" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D94" s="3">
-        <v>1.03229060576339</v>
+        <v>1.04700382111408</v>
       </c>
       <c r="E94" s="3">
-        <v>1.00726024942528</v>
+        <v>1.01880351165478</v>
       </c>
       <c r="F94" s="3">
-        <v>0.99586256046740596</v>
-      </c>
-      <c r="G94" s="3">
+        <v>1.02047205656197</v>
+      </c>
+      <c r="G94" s="4">
         <f t="shared" si="65"/>
-        <v>1.0116905466294543</v>
+        <v>1.0286791538663198</v>
       </c>
       <c r="H94" s="1"/>
       <c r="I94" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J94" s="3">
-        <v>0.973770179504438</v>
+        <v>0.96654889106271502</v>
       </c>
       <c r="K94" s="3">
-        <v>0.97016345061001896</v>
+        <v>0.96680702864797896</v>
       </c>
       <c r="L94" s="3">
-        <v>0.96386675207371497</v>
-      </c>
-      <c r="M94" s="3">
+        <v>0.97266608222409601</v>
+      </c>
+      <c r="M94" s="4">
         <f t="shared" si="66"/>
-        <v>0.96925814656936626</v>
+        <v>0.96866988749811656</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A95" s="4"/>
+      <c r="A95" s="5"/>
       <c r="B95" s="1"/>
       <c r="C95" s="2" t="s">
         <v>3</v>
@@ -3458,7 +4536,7 @@
       <c r="F95" s="3">
         <v>0.99382657677321895</v>
       </c>
-      <c r="G95" s="3">
+      <c r="G95" s="4">
         <f t="shared" si="65"/>
         <v>1.0107662482681545</v>
       </c>
@@ -3475,7 +4553,7 @@
       <c r="L95" s="3">
         <v>0.950471282950895</v>
       </c>
-      <c r="M95" s="3">
+      <c r="M95" s="4">
         <f t="shared" si="66"/>
         <v>0.9544333690059702</v>
       </c>
@@ -3484,40 +4562,40 @@
       <c r="C96" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D96" s="3">
+      <c r="D96" s="4">
         <f>GEOMEAN(D92:D95)</f>
-        <v>1.0290202520054583</v>
-      </c>
-      <c r="E96" s="3">
+        <v>1.0411389540548537</v>
+      </c>
+      <c r="E96" s="4">
         <f t="shared" ref="E96" si="67">GEOMEAN(E92:E95)</f>
-        <v>1.0053730951183801</v>
-      </c>
-      <c r="F96" s="3">
+        <v>1.0166761229789543</v>
+      </c>
+      <c r="F96" s="4">
         <f t="shared" ref="F96" si="68">GEOMEAN(F92:F95)</f>
-        <v>0.98924826824055367</v>
-      </c>
-      <c r="G96" s="3">
+        <v>1.0148808740983339</v>
+      </c>
+      <c r="G96" s="4">
         <f>GEOMEAN(G92:G95)</f>
-        <v>1.0077484988259613</v>
+        <v>1.0241623255952825</v>
       </c>
       <c r="I96" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J96" s="3">
+      <c r="J96" s="4">
         <f>GEOMEAN(J92:J95)</f>
-        <v>0.97112123821371521</v>
-      </c>
-      <c r="K96" s="3">
+        <v>0.96431657088615275</v>
+      </c>
+      <c r="K96" s="4">
         <f t="shared" ref="K96" si="69">GEOMEAN(K92:K95)</f>
-        <v>0.96186144805597096</v>
-      </c>
-      <c r="L96" s="3">
+        <v>0.96161729539523888</v>
+      </c>
+      <c r="L96" s="4">
         <f t="shared" ref="L96" si="70">GEOMEAN(L92:L95)</f>
-        <v>0.95369081788173926</v>
-      </c>
-      <c r="M96" s="3">
+        <v>0.96493748769712995</v>
+      </c>
+      <c r="M96" s="4">
         <f>GEOMEAN(M92:M95)</f>
-        <v>0.96219816408621106</v>
+        <v>0.96362270616725443</v>
       </c>
     </row>
   </sheetData>
@@ -3537,5 +4615,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed geometric mean issue and added code for 2nd dataset
Geometric means were not taken across all bottom levels of the hierarchy due to a typo previously.
</commit_message>
<xml_diff>
--- a/Accuracy rMAE and rRMSE (Cross-Sectional).xlsx
+++ b/Accuracy rMAE and rRMSE (Cross-Sectional).xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e00c848d2da39f20/Documents/3. Masters/Research/WindPowerForecasting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="618" documentId="8_{7CAE70F8-1326-4B7D-8A8A-809CD0BBBC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE315F62-DB23-4EBD-A571-397ADAD2A642}"/>
+  <xr:revisionPtr revIDLastSave="799" documentId="8_{7CAE70F8-1326-4B7D-8A8A-809CD0BBBC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D65488E-FA32-4D7B-A039-794424B44239}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{4F6B620E-8A72-45CF-9D17-FD2A4C076D11}"/>
+    <workbookView minimized="1" xWindow="1020" yWindow="1020" windowWidth="22610" windowHeight="15370" xr2:uid="{4F6B620E-8A72-45CF-9D17-FD2A4C076D11}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -105,8 +105,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -160,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -168,6 +169,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -253,25 +255,25 @@
             <c:numRef>
               <c:f>(Sheet1!$M$8,Sheet1!$M$16,Sheet1!$M$24,Sheet1!$M$32,Sheet1!$M$40,Sheet1!$M$48)</c:f>
               <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.96447067964771771</c:v>
+                  <c:v>0.96601105415054267</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.97352881698353588</c:v>
+                  <c:v>0.9673173083191845</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.95844563471779165</c:v>
+                  <c:v>0.95585596146827956</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.96778385588480964</c:v>
+                  <c:v>0.96342745441208977</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.9594888849411255</c:v>
+                  <c:v>0.95659543845051642</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.95530003781890815</c:v>
+                  <c:v>0.95188109798949605</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -331,22 +333,22 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.0309700880227557</c:v>
+                  <c:v>1.038578503379771</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0523003384247165</c:v>
+                  <c:v>1.0419225304376427</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.013318754775725</c:v>
+                  <c:v>1.0103146805899317</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0374231946797037</c:v>
+                  <c:v>1.0301866610845654</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.018162697334678</c:v>
+                  <c:v>1.014132678208207</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0147622801069813</c:v>
+                  <c:v>1.0101112990410712</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -355,110 +357,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-C4A2-4C2B-B295-FE65B603BC74}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>GB AvRelMAE</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>(Sheet1!$G$56,Sheet1!$G$64,Sheet1!$G$72,Sheet1!$G$80,Sheet1!$G$88,Sheet1!$G$96)</c:f>
-              <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1.0364136160503963</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0462386157374075</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.0313097689495503</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.0393989347860288</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.027878895513928</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.0241623255952825</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-BB80-4A83-8FE5-9A5DEF2879F5}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>GB AvRelRMSE</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>(Sheet1!$M$56,Sheet1!$M$64,Sheet1!$M$72,Sheet1!$M$80,Sheet1!$M$88,Sheet1!$M$96)</c:f>
-              <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.97202028869485435</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.970999859137338</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.97547640164003047</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.97331949246072047</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.96997165432465027</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.96362270616725443</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-BB80-4A83-8FE5-9A5DEF2879F5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -546,7 +444,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1261,10 +1159,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1564,28 +1458,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9C5127F-CD46-4E4E-96B7-010FB4E47685}">
   <dimension ref="A1:M96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X21" sqref="X21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="26.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7265625" customWidth="1"/>
-    <col min="5" max="5" width="12.26953125" customWidth="1"/>
+    <col min="1" max="2" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" customWidth="1"/>
     <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.26953125" customWidth="1"/>
-    <col min="11" max="11" width="11.7265625" customWidth="1"/>
+    <col min="7" max="7" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1796875" customWidth="1"/>
+    <col min="11" max="11" width="11.81640625" customWidth="1"/>
     <col min="12" max="12" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1604,7 +1498,7 @@
       <c r="L1" s="2"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="5"/>
+      <c r="A2" s="6"/>
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1617,7 +1511,7 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
+      <c r="A3" s="6"/>
       <c r="D3" s="2">
         <v>2</v>
       </c>
@@ -1644,7 +1538,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="5"/>
+      <c r="A4" s="6"/>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1652,7 +1546,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="3">
-        <v>1.0592846977557699</v>
+        <v>1.0407973260155801</v>
       </c>
       <c r="E4" s="3">
         <v>1.02963208908215</v>
@@ -1661,8 +1555,8 @@
         <v>1.01954223361298</v>
       </c>
       <c r="G4" s="4">
-        <f>GEOMEAN(D4:F4)</f>
-        <v>1.0360164776196741</v>
+        <f>((D4^25)*(E4^4)*F4)^(1/30)</f>
+        <v>1.0385870976514824</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>5</v>
@@ -1671,7 +1565,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="3">
-        <v>0.95786849255492901</v>
+        <v>0.95696990143113203</v>
       </c>
       <c r="K4" s="3">
         <v>0.96231137817143597</v>
@@ -1680,18 +1574,18 @@
         <v>0.963744194627697</v>
       </c>
       <c r="M4" s="4">
-        <f>GEOMEAN(J4:L4)</f>
-        <v>0.96130476414365063</v>
+        <f>((J4^25)*(K4^4)*L4)^(1/30)</f>
+        <v>0.95790558950078897</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" s="5"/>
+      <c r="A5" s="6"/>
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="3">
-        <v>1.0624669731016201</v>
+        <v>1.0476333876758299</v>
       </c>
       <c r="E5" s="3">
         <v>1.0345983790967499</v>
@@ -1700,15 +1594,15 @@
         <v>1.02254900769569</v>
       </c>
       <c r="G5" s="4">
-        <f t="shared" ref="G5:G7" si="0">GEOMEAN(D5:F5)</f>
-        <v>1.0397376919401935</v>
+        <f t="shared" ref="G5:G7" si="0">((D5^25)*(E5^4)*F5)^(1/30)</f>
+        <v>1.0450413764293769</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J5" s="3">
-        <v>0.97142227333357301</v>
+        <v>0.97203758928288697</v>
       </c>
       <c r="K5" s="3">
         <v>0.97546497471058602</v>
@@ -1717,18 +1611,18 @@
         <v>0.97708035678514105</v>
       </c>
       <c r="M5" s="4">
-        <f t="shared" ref="M5:M7" si="1">GEOMEAN(J5:L5)</f>
-        <v>0.97465296092529352</v>
+        <f t="shared" ref="M5:M7" si="1">((J5^25)*(K5^4)*L5)^(1/30)</f>
+        <v>0.97266162819874147</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="5"/>
+      <c r="A6" s="6"/>
       <c r="B6" s="1"/>
       <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="3">
-        <v>1.0586499521530099</v>
+        <v>1.04643379828476</v>
       </c>
       <c r="E6" s="3">
         <v>1.03327618887192</v>
@@ -1738,14 +1632,14 @@
       </c>
       <c r="G6" s="4">
         <f t="shared" si="0"/>
-        <v>1.0336363912819944</v>
+        <v>1.0434215621119374</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J6" s="3">
-        <v>0.96913220142851997</v>
+        <v>0.97211184991669297</v>
       </c>
       <c r="K6" s="3">
         <v>0.973162609996154</v>
@@ -1755,17 +1649,17 @@
       </c>
       <c r="M6" s="4">
         <f t="shared" si="1"/>
-        <v>0.96802136850832932</v>
+        <v>0.9719064538585811</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="5"/>
+      <c r="A7" s="6"/>
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="3">
-        <v>1.04108496048175</v>
+        <v>1.03057960659685</v>
       </c>
       <c r="E7" s="3">
         <v>1.01789000019496</v>
@@ -1775,14 +1669,14 @@
       </c>
       <c r="G7" s="4">
         <f t="shared" si="0"/>
-        <v>1.0146727995991616</v>
+        <v>1.027356329840418</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="J7" s="3">
-        <v>0.96101489056904099</v>
+        <v>0.96273665733300995</v>
       </c>
       <c r="K7" s="3">
         <v>0.96009676922210796</v>
@@ -1792,7 +1686,7 @@
       </c>
       <c r="M7" s="4">
         <f t="shared" si="1"/>
-        <v>0.95402569622407141</v>
+        <v>0.96165529634636193</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
@@ -1801,7 +1695,7 @@
       </c>
       <c r="D8" s="4">
         <f>GEOMEAN(D4:D7)</f>
-        <v>1.0553382353283558</v>
+        <v>1.0413391594003274</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" ref="E8:F8" si="2">GEOMEAN(E4:E7)</f>
@@ -1813,14 +1707,14 @@
       </c>
       <c r="G8" s="4">
         <f>GEOMEAN(G4:G7)</f>
-        <v>1.0309700880227557</v>
+        <v>1.038578503379771</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>20</v>
       </c>
       <c r="J8" s="4">
         <f>GEOMEAN(J4:J7)</f>
-        <v>0.96484326925716257</v>
+        <v>0.96594249148656341</v>
       </c>
       <c r="K8" s="4">
         <f t="shared" ref="K8" si="3">GEOMEAN(K4:K7)</f>
@@ -1830,13 +1724,13 @@
         <f t="shared" ref="L8" si="4">GEOMEAN(L4:L7)</f>
         <v>0.96084511344619006</v>
       </c>
-      <c r="M8" s="4">
+      <c r="M8" s="5">
         <f>GEOMEAN(M4:M7)</f>
-        <v>0.96447067964771771</v>
+        <v>0.96601105415054267</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1855,7 +1749,7 @@
       <c r="L9" s="2"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" s="5"/>
+      <c r="A10" s="6"/>
       <c r="D10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1868,7 +1762,7 @@
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" s="5"/>
+      <c r="A11" s="6"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2">
         <v>2</v>
@@ -1896,7 +1790,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" s="5"/>
+      <c r="A12" s="6"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1904,7 +1798,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="3">
-        <v>1.0592846977557699</v>
+        <v>1.0407973260155801</v>
       </c>
       <c r="E12" s="3">
         <v>1.04685597001332</v>
@@ -1913,8 +1807,8 @@
         <v>1.08688523187883</v>
       </c>
       <c r="G12" s="4">
-        <f>GEOMEAN(D12:F12)</f>
-        <v>1.0642110732152528</v>
+        <f>((D12^25)*(E12^4)*F12)^(1/30)</f>
+        <v>1.0431085870867398</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>5</v>
@@ -1923,7 +1817,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="3">
-        <v>0.95786849255492901</v>
+        <v>0.95696990143113203</v>
       </c>
       <c r="K12" s="3">
         <v>0.96598968370306104</v>
@@ -1932,18 +1826,18 @@
         <v>0.98561052417299899</v>
       </c>
       <c r="M12" s="4">
-        <f>GEOMEAN(J12:L12)</f>
-        <v>0.96975323318332907</v>
+        <f>((J12^25)*(K12^4)*L12)^(1/30)</f>
+        <v>0.95910997621467431</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" s="5"/>
+      <c r="A13" s="6"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="3">
-        <v>1.0624669731016201</v>
+        <v>1.0476333876758299</v>
       </c>
       <c r="E13" s="3">
         <v>1.04790841458322</v>
@@ -1952,15 +1846,15 @@
         <v>1.0752517632168599</v>
       </c>
       <c r="G13" s="4">
-        <f t="shared" ref="G13:G15" si="5">GEOMEAN(D13:F13)</f>
-        <v>1.0618169243800228</v>
+        <f t="shared" ref="G13:G15" si="5">((D13^25)*(E13^4)*F13)^(1/30)</f>
+        <v>1.0485791665488777</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J13" s="3">
-        <v>0.97142227333357301</v>
+        <v>0.97203758928288697</v>
       </c>
       <c r="K13" s="3">
         <v>0.98035084069364198</v>
@@ -1969,18 +1863,18 @@
         <v>1.0006159697182899</v>
       </c>
       <c r="M13" s="4">
-        <f t="shared" ref="M13:M15" si="6">GEOMEAN(J13:L13)</f>
-        <v>0.98405416576171734</v>
+        <f t="shared" ref="M13:M15" si="6">((J13^25)*(K13^4)*L13)^(1/30)</f>
+        <v>0.97408233499773156</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" s="5"/>
+      <c r="A14" s="6"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="3">
-        <v>1.0586499521530099</v>
+        <v>1.04643379828476</v>
       </c>
       <c r="E14" s="3">
         <v>1.0438183109836101</v>
@@ -1990,14 +1884,14 @@
       </c>
       <c r="G14" s="4">
         <f t="shared" si="5"/>
-        <v>1.0537253106790809</v>
+        <v>1.0464936998973637</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J14" s="3">
-        <v>0.96913220142851997</v>
+        <v>0.97211184991669297</v>
       </c>
       <c r="K14" s="3">
         <v>0.977871288832728</v>
@@ -2007,17 +1901,17 @@
       </c>
       <c r="M14" s="4">
         <f t="shared" si="6"/>
-        <v>0.97887505889922799</v>
+        <v>0.9734604822462618</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="5"/>
+      <c r="A15" s="6"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="3">
-        <v>1.04108496048175</v>
+        <v>1.03057960659685</v>
       </c>
       <c r="E15" s="3">
         <v>1.0251924034392199</v>
@@ -2027,14 +1921,14 @@
       </c>
       <c r="G15" s="4">
         <f t="shared" si="5"/>
-        <v>1.0298026651788392</v>
+        <v>1.0296137970056103</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="2" t="s">
         <v>3</v>
       </c>
       <c r="J15" s="3">
-        <v>0.96101489056904099</v>
+        <v>0.96273665733300995</v>
       </c>
       <c r="K15" s="3">
         <v>0.96300244811978197</v>
@@ -2044,7 +1938,7 @@
       </c>
       <c r="M15" s="4">
         <f t="shared" si="6"/>
-        <v>0.96158513739777274</v>
+        <v>0.9627054559415652</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
@@ -2053,7 +1947,7 @@
       </c>
       <c r="D16" s="4">
         <f>GEOMEAN(D12:D15)</f>
-        <v>1.0553382353283558</v>
+        <v>1.0413391594003274</v>
       </c>
       <c r="E16" s="4">
         <f t="shared" ref="E16" si="7">GEOMEAN(E12:E15)</f>
@@ -2065,14 +1959,14 @@
       </c>
       <c r="G16" s="4">
         <f>GEOMEAN(G12:G15)</f>
-        <v>1.0523003384247165</v>
+        <v>1.0419225304376427</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>20</v>
       </c>
       <c r="J16" s="4">
         <f>GEOMEAN(J12:J15)</f>
-        <v>0.96484326925716257</v>
+        <v>0.96594249148656341</v>
       </c>
       <c r="K16" s="4">
         <f t="shared" ref="K16" si="9">GEOMEAN(K12:K15)</f>
@@ -2082,13 +1976,13 @@
         <f t="shared" ref="L16" si="10">GEOMEAN(L12:L15)</f>
         <v>0.98406523101753762</v>
       </c>
-      <c r="M16" s="4">
+      <c r="M16" s="5">
         <f>GEOMEAN(M12:M15)</f>
-        <v>0.97352881698353588</v>
+        <v>0.9673173083191845</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -2107,7 +2001,7 @@
       <c r="L17" s="2"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" s="5"/>
+      <c r="A18" s="6"/>
       <c r="D18" s="1" t="s">
         <v>4</v>
       </c>
@@ -2120,7 +2014,7 @@
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" s="5"/>
+      <c r="A19" s="6"/>
       <c r="D19" s="2">
         <v>2</v>
       </c>
@@ -2147,7 +2041,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20" s="5"/>
+      <c r="A20" s="6"/>
       <c r="B20" s="1" t="s">
         <v>5</v>
       </c>
@@ -2155,7 +2049,7 @@
         <v>0</v>
       </c>
       <c r="D20" s="3">
-        <v>1.0228197397981</v>
+        <v>1.00396645928804</v>
       </c>
       <c r="E20" s="3">
         <v>1.00371689303388</v>
@@ -2164,8 +2058,8 @@
         <v>1.01954223361298</v>
       </c>
       <c r="G20" s="4">
-        <f>GEOMEAN(D20:F20)</f>
-        <v>1.0153252462482847</v>
+        <f>((D20^25)*(E20^4)*F20)^(1/30)</f>
+        <v>1.0044485015533891</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>5</v>
@@ -2174,7 +2068,7 @@
         <v>0</v>
       </c>
       <c r="J20" s="3">
-        <v>0.95144852670656799</v>
+        <v>0.94788089601007197</v>
       </c>
       <c r="K20" s="3">
         <v>0.95429728578715001</v>
@@ -2183,18 +2077,18 @@
         <v>0.963744194627697</v>
       </c>
       <c r="M20" s="4">
-        <f>GEOMEAN(J20:L20)</f>
-        <v>0.95648226218687182</v>
+        <f>((J20^25)*(K20^4)*L20)^(1/30)</f>
+        <v>0.94925893348828383</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A21" s="5"/>
+      <c r="A21" s="6"/>
       <c r="B21" s="1"/>
       <c r="C21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D21" s="3">
-        <v>1.03210039427949</v>
+        <v>1.01600523274077</v>
       </c>
       <c r="E21" s="3">
         <v>1.0123622894270901</v>
@@ -2203,15 +2097,15 @@
         <v>1.02254900769569</v>
       </c>
       <c r="G21" s="4">
-        <f t="shared" ref="G21:G23" si="11">GEOMEAN(D21:F21)</f>
-        <v>1.0223054552264137</v>
+        <f t="shared" ref="G21:G23" si="11">((D21^25)*(E21^4)*F21)^(1/30)</f>
+        <v>1.0157360961261033</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J21" s="3">
-        <v>0.963549379381616</v>
+        <v>0.96163145954583795</v>
       </c>
       <c r="K21" s="3">
         <v>0.96741125401856098</v>
@@ -2220,18 +2114,18 @@
         <v>0.97708035678514105</v>
       </c>
       <c r="M21" s="4">
-        <f t="shared" ref="M21:M23" si="12">GEOMEAN(J21:L21)</f>
-        <v>0.96933032108217998</v>
+        <f t="shared" ref="M21:M23" si="12">((J21^25)*(K21^4)*L21)^(1/30)</f>
+        <v>0.96291151382047191</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A22" s="5"/>
+      <c r="A22" s="6"/>
       <c r="B22" s="1"/>
       <c r="C22" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D22" s="3">
-        <v>1.0263982398206</v>
+        <v>1.0165734713030099</v>
       </c>
       <c r="E22" s="3">
         <v>1.0100643019183599</v>
@@ -2241,14 +2135,14 @@
       </c>
       <c r="G22" s="4">
         <f t="shared" si="11"/>
-        <v>1.0153127272489262</v>
+        <v>1.0154689894151665</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J22" s="3">
-        <v>0.95714153250074496</v>
+        <v>0.95884682463597704</v>
       </c>
       <c r="K22" s="3">
         <v>0.96162661993674803</v>
@@ -2258,17 +2152,17 @@
       </c>
       <c r="M22" s="4">
         <f t="shared" si="12"/>
-        <v>0.96018815516243883</v>
+        <v>0.95931544947673331</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A23" s="5"/>
+      <c r="A23" s="6"/>
       <c r="B23" s="1"/>
       <c r="C23" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D23" s="3">
-        <v>1.01498724616947</v>
+        <v>1.00724469561282</v>
       </c>
       <c r="E23" s="3">
         <v>1.0007930218911101</v>
@@ -2278,14 +2172,14 @@
       </c>
       <c r="G23" s="4">
         <f t="shared" si="11"/>
-        <v>1.0004574657383061</v>
+        <v>1.0056605819197706</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="2" t="s">
         <v>3</v>
       </c>
       <c r="J23" s="3">
-        <v>0.95163485840659801</v>
+        <v>0.95259673411731605</v>
       </c>
       <c r="K23" s="3">
         <v>0.95101897658663503</v>
@@ -2295,7 +2189,7 @@
       </c>
       <c r="M23" s="4">
         <f t="shared" si="12"/>
-        <v>0.94790512690806328</v>
+        <v>0.95200077292838148</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
@@ -2304,7 +2198,7 @@
       </c>
       <c r="D24" s="4">
         <f>GEOMEAN(D20:D23)</f>
-        <v>1.0240575933317637</v>
+        <v>1.0109326600382462</v>
       </c>
       <c r="E24" s="4">
         <f t="shared" ref="E24" si="13">GEOMEAN(E20:E23)</f>
@@ -2316,14 +2210,14 @@
       </c>
       <c r="G24" s="4">
         <f>GEOMEAN(G20:G23)</f>
-        <v>1.013318754775725</v>
+        <v>1.0103146805899317</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>20</v>
       </c>
       <c r="J24" s="4">
         <f>GEOMEAN(J20:J23)</f>
-        <v>0.95593077713820407</v>
+        <v>0.95522391941894547</v>
       </c>
       <c r="K24" s="4">
         <f t="shared" ref="K24" si="15">GEOMEAN(K20:K23)</f>
@@ -2333,13 +2227,13 @@
         <f t="shared" ref="L24" si="16">GEOMEAN(L20:L23)</f>
         <v>0.96084511344619006</v>
       </c>
-      <c r="M24" s="4">
+      <c r="M24" s="5">
         <f>GEOMEAN(M20:M23)</f>
-        <v>0.95844563471779165</v>
+        <v>0.95585596146827956</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -2358,7 +2252,7 @@
       <c r="L25" s="2"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A26" s="5"/>
+      <c r="A26" s="6"/>
       <c r="D26" s="1" t="s">
         <v>4</v>
       </c>
@@ -2371,7 +2265,7 @@
       <c r="L26" s="1"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A27" s="5"/>
+      <c r="A27" s="6"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2">
         <v>2</v>
@@ -2399,7 +2293,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A28" s="5"/>
+      <c r="A28" s="6"/>
       <c r="B28" s="1" t="s">
         <v>5</v>
       </c>
@@ -2407,7 +2301,7 @@
         <v>0</v>
       </c>
       <c r="D28" s="3">
-        <v>1.0451574791462701</v>
+        <v>1.0254528461602299</v>
       </c>
       <c r="E28" s="3">
         <v>1.02963208908215</v>
@@ -2416,8 +2310,8 @@
         <v>1.0564432832645301</v>
       </c>
       <c r="G28" s="4">
-        <f>GEOMEAN(D28:F28)</f>
-        <v>1.0436863320263041</v>
+        <f>((D28^25)*(E28^4)*F28)^(1/30)</f>
+        <v>1.0270278670651247</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>5</v>
@@ -2426,7 +2320,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="3">
-        <v>0.95540855624620002</v>
+        <v>0.95379360896931098</v>
       </c>
       <c r="K28" s="3">
         <v>0.96231137817143597</v>
@@ -2435,18 +2329,18 @@
         <v>0.97507127672308302</v>
       </c>
       <c r="M28" s="4">
-        <f>GEOMEAN(J28:L28)</f>
-        <v>0.96422940197681983</v>
+        <f>((J28^25)*(K28^4)*L28)^(1/30)</f>
+        <v>0.95562749125855695</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A29" s="5"/>
+      <c r="A29" s="6"/>
       <c r="B29" s="1"/>
       <c r="C29" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D29" s="3">
-        <v>1.05071023730076</v>
+        <v>1.0351070127675299</v>
       </c>
       <c r="E29" s="3">
         <v>1.0345983790967499</v>
@@ -2455,15 +2349,15 @@
         <v>1.05262441781215</v>
       </c>
       <c r="G29" s="4">
-        <f t="shared" ref="G29:G31" si="17">GEOMEAN(D29:F29)</f>
-        <v>1.0459463270126135</v>
+        <f t="shared" ref="G29:G31" si="17">((D29^25)*(E29^4)*F29)^(1/30)</f>
+        <v>1.0356183322071362</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J29" s="3">
-        <v>0.96840645966161498</v>
+        <v>0.96776499116727499</v>
       </c>
       <c r="K29" s="3">
         <v>0.97546497471058602</v>
@@ -2472,18 +2366,18 @@
         <v>0.98858558669989005</v>
       </c>
       <c r="M29" s="4">
-        <f t="shared" ref="M29:M31" si="18">GEOMEAN(J29:L29)</f>
-        <v>0.97744998443858488</v>
+        <f t="shared" ref="M29:M31" si="18">((J29^25)*(K29^4)*L29)^(1/30)</f>
+        <v>0.96947576282390036</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A30" s="5"/>
+      <c r="A30" s="6"/>
       <c r="B30" s="1"/>
       <c r="C30" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D30" s="3">
-        <v>1.0466996668292099</v>
+        <v>1.03640573573786</v>
       </c>
       <c r="E30" s="3">
         <v>1.03327618887192</v>
@@ -2493,14 +2387,14 @@
       </c>
       <c r="G30" s="4">
         <f t="shared" si="17"/>
-        <v>1.0397856301903527</v>
+        <v>1.0360883575320095</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J30" s="3">
-        <v>0.96538583662063304</v>
+        <v>0.96792764185481295</v>
       </c>
       <c r="K30" s="3">
         <v>0.973162609996154</v>
@@ -2510,17 +2404,17 @@
       </c>
       <c r="M30" s="4">
         <f t="shared" si="18"/>
-        <v>0.97210101413935612</v>
+        <v>0.96895154766648928</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A31" s="5"/>
+      <c r="A31" s="6"/>
       <c r="B31" s="1"/>
       <c r="C31" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D31" s="3">
-        <v>1.0332404987650501</v>
+        <v>1.0232218558450401</v>
       </c>
       <c r="E31" s="3">
         <v>1.01789000019496</v>
@@ -2530,14 +2424,14 @@
       </c>
       <c r="G31" s="4">
         <f t="shared" si="17"/>
-        <v>1.0204708615588414</v>
+        <v>1.0220801133892472</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="2" t="s">
         <v>3</v>
       </c>
       <c r="J31" s="3">
-        <v>0.95913027991099897</v>
+        <v>0.95993128490425605</v>
       </c>
       <c r="K31" s="3">
         <v>0.96009676922210796</v>
@@ -2547,7 +2441,7 @@
       </c>
       <c r="M31" s="4">
         <f t="shared" si="18"/>
-        <v>0.95747442442063202</v>
+        <v>0.95972856363907555</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
@@ -2556,7 +2450,7 @@
       </c>
       <c r="D32" s="4">
         <f>GEOMEAN(D28:D31)</f>
-        <v>1.0439316161691148</v>
+        <v>1.0300306321050972</v>
       </c>
       <c r="E32" s="4">
         <f t="shared" ref="E32" si="19">GEOMEAN(E28:E31)</f>
@@ -2568,14 +2462,14 @@
       </c>
       <c r="G32" s="4">
         <f>GEOMEAN(G28:G31)</f>
-        <v>1.0374231946797037</v>
+        <v>1.0301866610845654</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>20</v>
       </c>
       <c r="J32" s="4">
         <f>GEOMEAN(J28:J31)</f>
-        <v>0.96206924651663372</v>
+        <v>0.96233623461718021</v>
       </c>
       <c r="K32" s="4">
         <f t="shared" ref="K32" si="21">GEOMEAN(K28:K31)</f>
@@ -2585,13 +2479,13 @@
         <f t="shared" ref="L32" si="22">GEOMEAN(L28:L31)</f>
         <v>0.97358047646493007</v>
       </c>
-      <c r="M32" s="4">
+      <c r="M32" s="5">
         <f>GEOMEAN(M28:M31)</f>
-        <v>0.96778385588480964</v>
+        <v>0.96342745441208977</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -2610,7 +2504,7 @@
       <c r="L33" s="2"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A34" s="5"/>
+      <c r="A34" s="6"/>
       <c r="D34" s="1" t="s">
         <v>4</v>
       </c>
@@ -2623,7 +2517,7 @@
       <c r="L34" s="1"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A35" s="5"/>
+      <c r="A35" s="6"/>
       <c r="D35" s="2">
         <v>2</v>
       </c>
@@ -2650,7 +2544,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A36" s="5"/>
+      <c r="A36" s="6"/>
       <c r="B36" s="1" t="s">
         <v>5</v>
       </c>
@@ -2658,7 +2552,7 @@
         <v>0</v>
       </c>
       <c r="D36" s="3">
-        <v>1.02841013900781</v>
+        <v>1.00768895211067</v>
       </c>
       <c r="E36" s="3">
         <v>1.0063014214122601</v>
@@ -2667,8 +2561,8 @@
         <v>1.02662132634825</v>
       </c>
       <c r="G36" s="4">
-        <f>GEOMEAN(D36:F36)</f>
-        <v>1.0203948057283321</v>
+        <f>((D36^25)*(E36^4)*F36)^(1/30)</f>
+        <v>1.0081291406799948</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>5</v>
@@ -2677,7 +2571,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="3">
-        <v>0.95063087802887303</v>
+        <v>0.94794406836038103</v>
       </c>
       <c r="K36" s="3">
         <v>0.95405184589922698</v>
@@ -2686,18 +2580,18 @@
         <v>0.96497369232735397</v>
       </c>
       <c r="M36" s="4">
-        <f>GEOMEAN(J36:L36)</f>
-        <v>0.95653262823580587</v>
+        <f>((J36^25)*(K36^4)*L36)^(1/30)</f>
+        <v>0.94931943863461199</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A37" s="5"/>
+      <c r="A37" s="6"/>
       <c r="B37" s="1"/>
       <c r="C37" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D37" s="3">
-        <v>1.0372909143167199</v>
+        <v>1.0198174765474299</v>
       </c>
       <c r="E37" s="3">
         <v>1.0153450654570799</v>
@@ -2706,15 +2600,15 @@
         <v>1.0284804317546199</v>
       </c>
       <c r="G37" s="4">
-        <f t="shared" ref="G37:G39" si="23">GEOMEAN(D37:F37)</f>
-        <v>1.0269991634116376</v>
+        <f t="shared" ref="G37:G39" si="23">((D37^25)*(E37^4)*F37)^(1/30)</f>
+        <v>1.0195074363877985</v>
       </c>
       <c r="H37" s="1"/>
       <c r="I37" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J37" s="3">
-        <v>0.963669704838515</v>
+        <v>0.96200075364414195</v>
       </c>
       <c r="K37" s="3">
         <v>0.96782692161109696</v>
@@ -2723,18 +2617,18 @@
         <v>0.97853919737083295</v>
       </c>
       <c r="M37" s="4">
-        <f t="shared" ref="M37:M39" si="24">GEOMEAN(J37:L37)</f>
-        <v>0.96999175747240807</v>
+        <f t="shared" ref="M37:M39" si="24">((J37^25)*(K37^4)*L37)^(1/30)</f>
+        <v>0.96332273700436155</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A38" s="5"/>
+      <c r="A38" s="6"/>
       <c r="B38" s="1"/>
       <c r="C38" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D38" s="3">
-        <v>1.0328736856706799</v>
+        <v>1.0209767787572701</v>
       </c>
       <c r="E38" s="3">
         <v>1.01342860315996</v>
@@ -2744,14 +2638,14 @@
       </c>
       <c r="G38" s="4">
         <f t="shared" si="23"/>
-        <v>1.0205119752066012</v>
+        <v>1.0197790983621235</v>
       </c>
       <c r="H38" s="1"/>
       <c r="I38" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J38" s="3">
-        <v>0.95902719177627305</v>
+        <v>0.960247400366395</v>
       </c>
       <c r="K38" s="3">
         <v>0.96258651055766498</v>
@@ -2761,17 +2655,17 @@
       </c>
       <c r="M38" s="4">
         <f t="shared" si="24"/>
-        <v>0.96208972200007081</v>
+        <v>0.96070589151368602</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A39" s="5"/>
+      <c r="A39" s="6"/>
       <c r="B39" s="1"/>
       <c r="C39" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D39" s="3">
-        <v>1.020777598941</v>
+        <v>1.0108683022373699</v>
       </c>
       <c r="E39" s="3">
         <v>1.00324642511107</v>
@@ -2781,14 +2675,14 @@
       </c>
       <c r="G39" s="4">
         <f t="shared" si="23"/>
-        <v>1.004875579795937</v>
+        <v>1.0091748895256496</v>
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="2" t="s">
         <v>3</v>
       </c>
       <c r="J39" s="3">
-        <v>0.95327699141563005</v>
+        <v>0.95370091164280302</v>
       </c>
       <c r="K39" s="3">
         <v>0.95180396132658296</v>
@@ -2798,7 +2692,7 @@
       </c>
       <c r="M39" s="4">
         <f t="shared" si="24"/>
-        <v>0.94945936942928222</v>
+        <v>0.95310025052402225</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.35">
@@ -2807,7 +2701,7 @@
       </c>
       <c r="D40" s="4">
         <f>GEOMEAN(D36:D39)</f>
-        <v>1.0298199879930348</v>
+        <v>1.0148219393315625</v>
       </c>
       <c r="E40" s="4">
         <f t="shared" ref="E40" si="25">GEOMEAN(E36:E39)</f>
@@ -2819,14 +2713,14 @@
       </c>
       <c r="G40" s="4">
         <f>GEOMEAN(G36:G39)</f>
-        <v>1.018162697334678</v>
+        <v>1.014132678208207</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>20</v>
       </c>
       <c r="J40" s="4">
         <f>GEOMEAN(J36:J39)</f>
-        <v>0.9566378031095315</v>
+        <v>0.95595701806609523</v>
       </c>
       <c r="K40" s="4">
         <f t="shared" ref="K40" si="27">GEOMEAN(K36:K39)</f>
@@ -2836,13 +2730,13 @@
         <f t="shared" ref="L40" si="28">GEOMEAN(L36:L39)</f>
         <v>0.96279331692144232</v>
       </c>
-      <c r="M40" s="4">
+      <c r="M40" s="5">
         <f>GEOMEAN(M36:M39)</f>
-        <v>0.9594888849411255</v>
+        <v>0.95659543845051642</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -2861,7 +2755,7 @@
       <c r="L41" s="2"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A42" s="5"/>
+      <c r="A42" s="6"/>
       <c r="D42" s="1" t="s">
         <v>4</v>
       </c>
@@ -2874,7 +2768,7 @@
       <c r="L42" s="1"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A43" s="5"/>
+      <c r="A43" s="6"/>
       <c r="D43" s="2">
         <v>2</v>
       </c>
@@ -2901,7 +2795,7 @@
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A44" s="5"/>
+      <c r="A44" s="6"/>
       <c r="B44" s="1" t="s">
         <v>5</v>
       </c>
@@ -2909,7 +2803,7 @@
         <v>0</v>
       </c>
       <c r="D44" s="3">
-        <v>1.0252949285986499</v>
+        <v>1.00391517455712</v>
       </c>
       <c r="E44" s="3">
         <v>1.0028969133834</v>
@@ -2918,8 +2812,8 @@
         <v>1.02192412461684</v>
       </c>
       <c r="G44" s="4">
-        <f>GEOMEAN(D44:F44)</f>
-        <v>1.0166573042097149</v>
+        <f>((D44^25)*(E44^4)*F44)^(1/30)</f>
+        <v>1.0043744200916631</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>5</v>
@@ -2928,7 +2822,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="3">
-        <v>0.94857968695696704</v>
+        <v>0.94467857442970105</v>
       </c>
       <c r="K44" s="3">
         <v>0.94986019613639705</v>
@@ -2937,18 +2831,18 @@
         <v>0.96414048159349297</v>
       </c>
       <c r="M44" s="4">
-        <f>GEOMEAN(J44:L44)</f>
-        <v>0.95416747628198195</v>
+        <f>((J44^25)*(K44^4)*L44)^(1/30)</f>
+        <v>0.94601064591395678</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A45" s="5"/>
+      <c r="A45" s="6"/>
       <c r="B45" s="1"/>
       <c r="C45" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D45" s="3">
-        <v>1.0346255048737201</v>
+        <v>1.0158351211047401</v>
       </c>
       <c r="E45" s="3">
         <v>1.01239308989587</v>
@@ -2957,15 +2851,15 @@
         <v>1.0253365206937</v>
       </c>
       <c r="G45" s="4">
-        <f t="shared" ref="G45:G47" si="29">GEOMEAN(D45:F45)</f>
-        <v>1.0240777402949637</v>
+        <f t="shared" ref="G45:G47" si="29">((D45^25)*(E45^4)*F45)^(1/30)</f>
+        <v>1.0156906559319023</v>
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J45" s="3">
-        <v>0.95813276472404296</v>
+        <v>0.95729913799553101</v>
       </c>
       <c r="K45" s="3">
         <v>0.96198902394411301</v>
@@ -2974,18 +2868,18 @@
         <v>0.97686064041802501</v>
       </c>
       <c r="M45" s="4">
-        <f t="shared" ref="M45:M47" si="30">GEOMEAN(J45:L45)</f>
-        <v>0.96562716170079643</v>
+        <f t="shared" ref="M45:M47" si="30">((J45^25)*(K45^4)*L45)^(1/30)</f>
+        <v>0.95856924864236659</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A46" s="5"/>
+      <c r="A46" s="6"/>
       <c r="B46" s="1"/>
       <c r="C46" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D46" s="3">
-        <v>1.0307590369843</v>
+        <v>1.0159543228993</v>
       </c>
       <c r="E46" s="3">
         <v>1.0099022198748799</v>
@@ -2995,14 +2889,14 @@
       </c>
       <c r="G46" s="4">
         <f t="shared" si="29"/>
-        <v>1.0175420029583118</v>
+        <v>1.0150164506120616</v>
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J46" s="3">
-        <v>0.95346949384957302</v>
+        <v>0.95434863907331402</v>
       </c>
       <c r="K46" s="3">
         <v>0.95571689914513103</v>
@@ -3012,17 +2906,17 @@
       </c>
       <c r="M46" s="4">
         <f t="shared" si="30"/>
-        <v>0.95728543729748417</v>
+        <v>0.95480802484592009</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A47" s="5"/>
+      <c r="A47" s="6"/>
       <c r="B47" s="1"/>
       <c r="C47" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D47" s="3">
-        <v>1.0134148267401899</v>
+        <v>1.00693524758553</v>
       </c>
       <c r="E47" s="3">
         <v>0.99996814849889104</v>
@@ -3032,14 +2926,14 @@
       </c>
       <c r="G47" s="4">
         <f t="shared" si="29"/>
-        <v>1.0009154789243422</v>
+        <v>1.0054181826791222</v>
       </c>
       <c r="H47" s="1"/>
       <c r="I47" s="2" t="s">
         <v>3</v>
       </c>
       <c r="J47" s="3">
-        <v>0.94491793410518898</v>
+        <v>0.94877946089843201</v>
       </c>
       <c r="K47" s="3">
         <v>0.94614154500927405</v>
@@ -3049,7 +2943,7 @@
       </c>
       <c r="M47" s="4">
         <f t="shared" si="30"/>
-        <v>0.94424271972621476</v>
+        <v>0.94818970325408125</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.35">
@@ -3058,7 +2952,7 @@
       </c>
       <c r="D48" s="4">
         <f>GEOMEAN(D44:D47)</f>
-        <v>1.0259922932869916</v>
+        <v>1.0106458388375112</v>
       </c>
       <c r="E48" s="4">
         <f t="shared" ref="E48" si="31">GEOMEAN(E44:E47)</f>
@@ -3070,14 +2964,14 @@
       </c>
       <c r="G48" s="4">
         <f>GEOMEAN(G44:G47)</f>
-        <v>1.0147622801069813</v>
+        <v>1.0101112990410712</v>
       </c>
       <c r="I48" s="2" t="s">
         <v>20</v>
       </c>
       <c r="J48" s="4">
         <f>GEOMEAN(J44:J47)</f>
-        <v>0.95126189751231793</v>
+        <v>0.95126390180214748</v>
       </c>
       <c r="K48" s="4">
         <f t="shared" ref="K48" si="33">GEOMEAN(K44:K47)</f>
@@ -3087,13 +2981,13 @@
         <f t="shared" ref="L48" si="34">GEOMEAN(L44:L47)</f>
         <v>0.96125915108596383</v>
       </c>
-      <c r="M48" s="4">
+      <c r="M48" s="5">
         <f>GEOMEAN(M44:M47)</f>
-        <v>0.95530003781890815</v>
+        <v>0.95188109798949605</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A49" s="5" t="s">
+      <c r="A49" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B49" s="2" t="s">
@@ -3112,7 +3006,7 @@
       <c r="L49" s="2"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A50" s="5"/>
+      <c r="A50" s="6"/>
       <c r="D50" s="1" t="s">
         <v>4</v>
       </c>
@@ -3125,7 +3019,7 @@
       <c r="L50" s="1"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A51" s="5"/>
+      <c r="A51" s="6"/>
       <c r="D51" s="2">
         <v>2</v>
       </c>
@@ -3152,7 +3046,7 @@
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A52" s="5"/>
+      <c r="A52" s="6"/>
       <c r="B52" s="1" t="s">
         <v>5</v>
       </c>
@@ -3160,7 +3054,7 @@
         <v>0</v>
       </c>
       <c r="D52" s="3">
-        <v>1.0692381859906299</v>
+        <v>1.0562373267640499</v>
       </c>
       <c r="E52" s="3">
         <v>1.0373160385958999</v>
@@ -3170,7 +3064,7 @@
       </c>
       <c r="G52" s="4">
         <f>GEOMEAN(D52:F52)</f>
-        <v>1.0430936303680722</v>
+        <v>1.0388487230751855</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>5</v>
@@ -3179,7 +3073,7 @@
         <v>0</v>
       </c>
       <c r="J52" s="3">
-        <v>0.96812571259787406</v>
+        <v>0.96441060139877</v>
       </c>
       <c r="K52" s="3">
         <v>0.96707352322590001</v>
@@ -3189,17 +3083,17 @@
       </c>
       <c r="M52" s="4">
         <f>GEOMEAN(J52:L52)</f>
-        <v>0.96625461618062802</v>
+        <v>0.96501705480977207</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A53" s="5"/>
+      <c r="A53" s="6"/>
       <c r="B53" s="1"/>
       <c r="C53" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D53" s="3">
-        <v>1.0711509833739401</v>
+        <v>1.0559532854573701</v>
       </c>
       <c r="E53" s="3">
         <v>1.0357229311486</v>
@@ -3209,14 +3103,14 @@
       </c>
       <c r="G53" s="4">
         <f t="shared" ref="G53:G55" si="35">GEOMEAN(D53:F53)</f>
-        <v>1.0436076413229503</v>
+        <v>1.0386484771048679</v>
       </c>
       <c r="H53" s="1"/>
       <c r="I53" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J53" s="3">
-        <v>0.97782040839761697</v>
+        <v>0.97607512061208102</v>
       </c>
       <c r="K53" s="3">
         <v>0.97793251173983098</v>
@@ -3226,17 +3120,17 @@
       </c>
       <c r="M53" s="4">
         <f t="shared" ref="M53:M55" si="36">GEOMEAN(J53:L53)</f>
-        <v>0.97975382961618729</v>
+        <v>0.97917056956224924</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A54" s="5"/>
+      <c r="A54" s="6"/>
       <c r="B54" s="1"/>
       <c r="C54" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D54" s="3">
-        <v>1.0665521648848599</v>
+        <v>1.054412563718</v>
       </c>
       <c r="E54" s="3">
         <v>1.0356716865346001</v>
@@ -3246,14 +3140,14 @@
       </c>
       <c r="G54" s="4">
         <f t="shared" si="35"/>
-        <v>1.0409760439932174</v>
+        <v>1.0370114669094932</v>
       </c>
       <c r="H54" s="1"/>
       <c r="I54" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J54" s="3">
-        <v>0.97460928398468805</v>
+        <v>0.97671705058722402</v>
       </c>
       <c r="K54" s="3">
         <v>0.98008723465191205</v>
@@ -3263,17 +3157,17 @@
       </c>
       <c r="M54" s="4">
         <f t="shared" si="36"/>
-        <v>0.97731425279212136</v>
+        <v>0.97801828436463956</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A55" s="5"/>
+      <c r="A55" s="6"/>
       <c r="B55" s="1"/>
       <c r="C55" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D55" s="3">
-        <v>1.0428642074413801</v>
+        <v>1.0382703098046899</v>
       </c>
       <c r="E55" s="3">
         <v>1.0265770752832999</v>
@@ -3283,14 +3177,14 @@
       </c>
       <c r="G55" s="4">
         <f t="shared" si="35"/>
-        <v>1.0181954709349592</v>
+        <v>1.0166981935901345</v>
       </c>
       <c r="H55" s="1"/>
       <c r="I55" s="2" t="s">
         <v>3</v>
       </c>
       <c r="J55" s="3">
-        <v>0.96364752563588796</v>
+        <v>0.97164173836739698</v>
       </c>
       <c r="K55" s="3">
         <v>0.97077699455370903</v>
@@ -3300,7 +3194,7 @@
       </c>
       <c r="M55" s="4">
         <f t="shared" si="36"/>
-        <v>0.96484718888082177</v>
+        <v>0.96750789978663387</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.35">
@@ -3309,7 +3203,7 @@
       </c>
       <c r="D56" s="4">
         <f>GEOMEAN(D52:D55)</f>
-        <v>1.062389460846165</v>
+        <v>1.0511914165836065</v>
       </c>
       <c r="E56" s="4">
         <f t="shared" ref="E56" si="37">GEOMEAN(E52:E55)</f>
@@ -3321,14 +3215,14 @@
       </c>
       <c r="G56" s="4">
         <f>GEOMEAN(G52:G55)</f>
-        <v>1.0364136160503963</v>
+        <v>1.032759330692262</v>
       </c>
       <c r="I56" s="2" t="s">
         <v>20</v>
       </c>
       <c r="J56" s="4">
         <f>GEOMEAN(J52:J55)</f>
-        <v>0.97103503977214545</v>
+        <v>0.97219870358874638</v>
       </c>
       <c r="K56" s="4">
         <f t="shared" ref="K56" si="39">GEOMEAN(K52:K55)</f>
@@ -3338,13 +3232,13 @@
         <f t="shared" ref="L56" si="40">GEOMEAN(L52:L55)</f>
         <v>0.97107537555769785</v>
       </c>
-      <c r="M56" s="4">
+      <c r="M56" s="5">
         <f>GEOMEAN(M52:M55)</f>
-        <v>0.97202028869485435</v>
+        <v>0.97240841520044896</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A57" s="5" t="s">
+      <c r="A57" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B57" s="2" t="s">
@@ -3363,7 +3257,7 @@
       <c r="L57" s="2"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A58" s="5"/>
+      <c r="A58" s="6"/>
       <c r="D58" s="1" t="s">
         <v>4</v>
       </c>
@@ -3376,7 +3270,7 @@
       <c r="L58" s="1"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A59" s="5"/>
+      <c r="A59" s="6"/>
       <c r="D59" s="2">
         <v>2</v>
       </c>
@@ -3403,7 +3297,7 @@
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A60" s="5"/>
+      <c r="A60" s="6"/>
       <c r="B60" s="1" t="s">
         <v>5</v>
       </c>
@@ -3411,7 +3305,7 @@
         <v>0</v>
       </c>
       <c r="D60" s="3">
-        <v>1.0692381859906299</v>
+        <v>1.0562373267640499</v>
       </c>
       <c r="E60" s="3">
         <v>1.0446037868689699</v>
@@ -3421,7 +3315,7 @@
       </c>
       <c r="G60" s="4">
         <f>GEOMEAN(D60:F60)</f>
-        <v>1.0594413852308702</v>
+        <v>1.0551299501577163</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>5</v>
@@ -3430,7 +3324,7 @@
         <v>0</v>
       </c>
       <c r="J60" s="3">
-        <v>0.96812571259787406</v>
+        <v>0.96441060139877</v>
       </c>
       <c r="K60" s="3">
         <v>0.96004000335051898</v>
@@ -3440,17 +3334,17 @@
       </c>
       <c r="M60" s="4">
         <f>GEOMEAN(J60:L60)</f>
-        <v>0.96588391302539334</v>
+        <v>0.9646468264444088</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A61" s="5"/>
+      <c r="A61" s="6"/>
       <c r="B61" s="1"/>
       <c r="C61" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D61" s="3">
-        <v>1.0711509833739401</v>
+        <v>1.0559532854573701</v>
       </c>
       <c r="E61" s="3">
         <v>1.0426158574501001</v>
@@ -3460,14 +3354,14 @@
       </c>
       <c r="G61" s="4">
         <f t="shared" ref="G61:G63" si="41">GEOMEAN(D61:F61)</f>
-        <v>1.0548217757614406</v>
+        <v>1.0498093226136473</v>
       </c>
       <c r="H61" s="1"/>
       <c r="I61" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J61" s="3">
-        <v>0.97782040839761697</v>
+        <v>0.97607512061208102</v>
       </c>
       <c r="K61" s="3">
         <v>0.973761303851023</v>
@@ -3477,17 +3371,17 @@
       </c>
       <c r="M61" s="4">
         <f t="shared" ref="M61:M63" si="42">GEOMEAN(J61:L61)</f>
-        <v>0.97896963493389888</v>
+        <v>0.97838684172113954</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A62" s="5"/>
+      <c r="A62" s="6"/>
       <c r="B62" s="1"/>
       <c r="C62" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D62" s="3">
-        <v>1.0665521648848599</v>
+        <v>1.054412563718</v>
       </c>
       <c r="E62" s="3">
         <v>1.03834990632317</v>
@@ -3497,14 +3391,14 @@
       </c>
       <c r="G62" s="4">
         <f t="shared" si="41"/>
-        <v>1.0484472990085429</v>
+        <v>1.0444542675078399</v>
       </c>
       <c r="H62" s="1"/>
       <c r="I62" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J62" s="3">
-        <v>0.97460928398468805</v>
+        <v>0.97671705058722402</v>
       </c>
       <c r="K62" s="3">
         <v>0.97395690018127301</v>
@@ -3514,17 +3408,17 @@
       </c>
       <c r="M62" s="4">
         <f t="shared" si="42"/>
-        <v>0.97673812723768083</v>
+        <v>0.97744174378444959</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A63" s="5"/>
+      <c r="A63" s="6"/>
       <c r="B63" s="1"/>
       <c r="C63" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D63" s="3">
-        <v>1.0428642074413801</v>
+        <v>1.0382703098046899</v>
       </c>
       <c r="E63" s="3">
         <v>1.02003349513228</v>
@@ -3534,14 +3428,14 @@
       </c>
       <c r="G63" s="4">
         <f t="shared" si="41"/>
-        <v>1.0226343012112742</v>
+        <v>1.0211304964753933</v>
       </c>
       <c r="H63" s="1"/>
       <c r="I63" s="2" t="s">
         <v>3</v>
       </c>
       <c r="J63" s="3">
-        <v>0.96364752563588796</v>
+        <v>0.97164173836739698</v>
       </c>
       <c r="K63" s="3">
         <v>0.96428154271273803</v>
@@ -3551,7 +3445,7 @@
       </c>
       <c r="M63" s="4">
         <f t="shared" si="42"/>
-        <v>0.96250805467614375</v>
+        <v>0.96516231506838202</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.35">
@@ -3560,7 +3454,7 @@
       </c>
       <c r="D64" s="4">
         <f>GEOMEAN(D60:D63)</f>
-        <v>1.062389460846165</v>
+        <v>1.0511914165836065</v>
       </c>
       <c r="E64" s="4">
         <f t="shared" ref="E64" si="43">GEOMEAN(E60:E63)</f>
@@ -3572,14 +3466,14 @@
       </c>
       <c r="G64" s="4">
         <f>GEOMEAN(G60:G63)</f>
-        <v>1.0462386157374075</v>
+        <v>1.042549688464169</v>
       </c>
       <c r="I64" s="2" t="s">
         <v>20</v>
       </c>
       <c r="J64" s="4">
         <f>GEOMEAN(J60:J63)</f>
-        <v>0.97103503977214545</v>
+        <v>0.97219870358874638</v>
       </c>
       <c r="K64" s="4">
         <f t="shared" ref="K64" si="45">GEOMEAN(K60:K63)</f>
@@ -3589,13 +3483,13 @@
         <f t="shared" ref="L64" si="46">GEOMEAN(L60:L63)</f>
         <v>0.97398269410359695</v>
       </c>
-      <c r="M64" s="4">
+      <c r="M64" s="5">
         <f>GEOMEAN(M60:M63)</f>
-        <v>0.970999859137338</v>
+        <v>0.97138757818666543</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A65" s="5" t="s">
+      <c r="A65" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B65" s="2" t="s">
@@ -3614,7 +3508,7 @@
       <c r="L65" s="2"/>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A66" s="5"/>
+      <c r="A66" s="6"/>
       <c r="D66" s="1" t="s">
         <v>4</v>
       </c>
@@ -3627,7 +3521,7 @@
       <c r="L66" s="1"/>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A67" s="5"/>
+      <c r="A67" s="6"/>
       <c r="D67" s="2">
         <v>2</v>
       </c>
@@ -3654,7 +3548,7 @@
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A68" s="5"/>
+      <c r="A68" s="6"/>
       <c r="B68" s="1" t="s">
         <v>5</v>
       </c>
@@ -3662,7 +3556,7 @@
         <v>0</v>
       </c>
       <c r="D68" s="3">
-        <v>1.05528639170465</v>
+        <v>1.04480378637321</v>
       </c>
       <c r="E68" s="3">
         <v>1.0273873034579499</v>
@@ -3672,7 +3566,7 @@
       </c>
       <c r="G68" s="4">
         <f>GEOMEAN(D68:F68)</f>
-        <v>1.0352127677125957</v>
+        <v>1.0317736197642557</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>5</v>
@@ -3681,7 +3575,7 @@
         <v>0</v>
       </c>
       <c r="J68" s="3">
-        <v>0.97384506446603503</v>
+        <v>0.97257765500530902</v>
       </c>
       <c r="K68" s="3">
         <v>0.96859926003090802</v>
@@ -3691,17 +3585,17 @@
       </c>
       <c r="M68" s="4">
         <f>GEOMEAN(J68:L68)</f>
-        <v>0.96866252693817845</v>
+        <v>0.96824212295610401</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A69" s="5"/>
+      <c r="A69" s="6"/>
       <c r="B69" s="1"/>
       <c r="C69" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D69" s="3">
-        <v>1.06051822386519</v>
+        <v>1.0471617199056</v>
       </c>
       <c r="E69" s="3">
         <v>1.0290406582837901</v>
@@ -3711,14 +3605,14 @@
       </c>
       <c r="G69" s="4">
         <f t="shared" ref="G69:G71" si="47">GEOMEAN(D69:F69)</f>
-        <v>1.0379012768933922</v>
+        <v>1.0335256361075031</v>
       </c>
       <c r="H69" s="1"/>
       <c r="I69" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J69" s="3">
-        <v>0.98870407973306995</v>
+        <v>0.98430733435783802</v>
       </c>
       <c r="K69" s="3">
         <v>0.98229246896209699</v>
@@ -3728,17 +3622,17 @@
       </c>
       <c r="M69" s="4">
         <f t="shared" ref="M69:M71" si="48">GEOMEAN(J69:L69)</f>
-        <v>0.98483473094659624</v>
+        <v>0.98337271546123972</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A70" s="5"/>
+      <c r="A70" s="6"/>
       <c r="B70" s="1"/>
       <c r="C70" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D70" s="3">
-        <v>1.0561804240519901</v>
+        <v>1.05126718476655</v>
       </c>
       <c r="E70" s="3">
         <v>1.0329765565644999</v>
@@ -3748,14 +3642,14 @@
       </c>
       <c r="G70" s="4">
         <f t="shared" si="47"/>
-        <v>1.0366898818797889</v>
+        <v>1.0350798589573524</v>
       </c>
       <c r="H70" s="1"/>
       <c r="I70" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J70" s="3">
-        <v>0.980326215102578</v>
+        <v>0.98436647134438804</v>
       </c>
       <c r="K70" s="3">
         <v>0.98309358377894696</v>
@@ -3765,17 +3659,17 @@
       </c>
       <c r="M70" s="4">
         <f t="shared" si="48"/>
-        <v>0.98022167034575891</v>
+        <v>0.98156643308587599</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A71" s="5"/>
+      <c r="A71" s="6"/>
       <c r="B71" s="1"/>
       <c r="C71" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D71" s="3">
-        <v>1.0379241778057899</v>
+        <v>1.0407231381306901</v>
       </c>
       <c r="E71" s="3">
         <v>1.0235904231319</v>
@@ -3785,14 +3679,14 @@
       </c>
       <c r="G71" s="4">
         <f t="shared" si="47"/>
-        <v>1.0155983824502794</v>
+        <v>1.0165104812460359</v>
       </c>
       <c r="H71" s="1"/>
       <c r="I71" s="2" t="s">
         <v>3</v>
       </c>
       <c r="J71" s="3">
-        <v>0.96989749838399497</v>
+        <v>0.98202025056881603</v>
       </c>
       <c r="K71" s="3">
         <v>0.97489307774322098</v>
@@ -3802,7 +3696,7 @@
       </c>
       <c r="M71" s="4">
         <f t="shared" si="48"/>
-        <v>0.96829327509781937</v>
+        <v>0.972310816544109</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.35">
@@ -3811,7 +3705,7 @@
       </c>
       <c r="D72" s="4">
         <f>GEOMEAN(D68:D71)</f>
-        <v>1.0524417159171073</v>
+        <v>1.0459819820260932</v>
       </c>
       <c r="E72" s="4">
         <f t="shared" ref="E72" si="49">GEOMEAN(E68:E71)</f>
@@ -3823,14 +3717,14 @@
       </c>
       <c r="G72" s="4">
         <f>GEOMEAN(G68:G71)</f>
-        <v>1.0313097689495503</v>
+        <v>1.0291954274978687</v>
       </c>
       <c r="I72" s="2" t="s">
         <v>20</v>
       </c>
       <c r="J72" s="4">
         <f>GEOMEAN(J68:J71)</f>
-        <v>0.97816734955117812</v>
+        <v>0.98080589224263859</v>
       </c>
       <c r="K72" s="4">
         <f t="shared" ref="K72" si="51">GEOMEAN(K68:K71)</f>
@@ -3840,13 +3734,13 @@
         <f t="shared" ref="L72" si="52">GEOMEAN(L68:L71)</f>
         <v>0.97107537555769785</v>
       </c>
-      <c r="M72" s="4">
+      <c r="M72" s="5">
         <f>GEOMEAN(M68:M71)</f>
-        <v>0.97547640164003047</v>
+        <v>0.97635270886275727</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A73" s="5" t="s">
+      <c r="A73" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B73" s="2" t="s">
@@ -3865,7 +3759,7 @@
       <c r="L73" s="2"/>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A74" s="5"/>
+      <c r="A74" s="6"/>
       <c r="D74" s="1" t="s">
         <v>4</v>
       </c>
@@ -3878,7 +3772,7 @@
       <c r="L74" s="1"/>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A75" s="5"/>
+      <c r="A75" s="6"/>
       <c r="D75" s="2">
         <v>2</v>
       </c>
@@ -3905,7 +3799,7 @@
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A76" s="5"/>
+      <c r="A76" s="6"/>
       <c r="B76" s="1" t="s">
         <v>5</v>
       </c>
@@ -3913,7 +3807,7 @@
         <v>0</v>
       </c>
       <c r="D76" s="3">
-        <v>1.06491700073463</v>
+        <v>1.0512792327485601</v>
       </c>
       <c r="E76" s="3">
         <v>1.0373160385958999</v>
@@ -3923,7 +3817,7 @@
       </c>
       <c r="G76" s="4">
         <f>GEOMEAN(D76:F76)</f>
-        <v>1.0484549908751406</v>
+        <v>1.0439600985417272</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>5</v>
@@ -3932,7 +3826,7 @@
         <v>0</v>
       </c>
       <c r="J76" s="3">
-        <v>0.97499139368472798</v>
+        <v>0.97049735544774995</v>
       </c>
       <c r="K76" s="3">
         <v>0.96707352322590001</v>
@@ -3942,17 +3836,17 @@
       </c>
       <c r="M76" s="4">
         <f>GEOMEAN(J76:L76)</f>
-        <v>0.96794908170869476</v>
+        <v>0.9664595981840115</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A77" s="5"/>
+      <c r="A77" s="6"/>
       <c r="B77" s="1"/>
       <c r="C77" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D77" s="3">
-        <v>1.07170009126761</v>
+        <v>1.0523946374792701</v>
       </c>
       <c r="E77" s="3">
         <v>1.0357229311486</v>
@@ -3962,14 +3856,14 @@
       </c>
       <c r="G77" s="4">
         <f t="shared" ref="G77:G79" si="53">GEOMEAN(D77:F77)</f>
-        <v>1.046006966630131</v>
+        <v>1.0396879965206993</v>
       </c>
       <c r="H77" s="1"/>
       <c r="I77" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J77" s="3">
-        <v>0.988581174720222</v>
+        <v>0.98029969402296002</v>
       </c>
       <c r="K77" s="3">
         <v>0.97793251173983098</v>
@@ -3979,17 +3873,17 @@
       </c>
       <c r="M77" s="4">
         <f t="shared" ref="M77:M79" si="54">GEOMEAN(J77:L77)</f>
-        <v>0.98095013485992444</v>
+        <v>0.97820326541126124</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A78" s="5"/>
+      <c r="A78" s="6"/>
       <c r="B78" s="1"/>
       <c r="C78" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D78" s="3">
-        <v>1.0645365735836401</v>
+        <v>1.0536195130419299</v>
       </c>
       <c r="E78" s="3">
         <v>1.0356716865346001</v>
@@ -3999,14 +3893,14 @@
       </c>
       <c r="G78" s="4">
         <f t="shared" si="53"/>
-        <v>1.0412661254658415</v>
+        <v>1.0376944156384513</v>
       </c>
       <c r="H78" s="1"/>
       <c r="I78" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J78" s="3">
-        <v>0.98212471393134704</v>
+        <v>0.98164417408904903</v>
       </c>
       <c r="K78" s="3">
         <v>0.98008723465191205</v>
@@ -4016,17 +3910,17 @@
       </c>
       <c r="M78" s="4">
         <f t="shared" si="54"/>
-        <v>0.97905203240516314</v>
+        <v>0.97889232754776823</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A79" s="5"/>
+      <c r="A79" s="6"/>
       <c r="B79" s="1"/>
       <c r="C79" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D79" s="3">
-        <v>1.0462322259069601</v>
+        <v>1.0429987945985399</v>
       </c>
       <c r="E79" s="3">
         <v>1.0265770752832999</v>
@@ -4036,14 +3930,14 @@
       </c>
       <c r="G79" s="4">
         <f t="shared" si="53"/>
-        <v>1.0220754601760698</v>
+        <v>1.0210214490533014</v>
       </c>
       <c r="H79" s="1"/>
       <c r="I79" s="2" t="s">
         <v>3</v>
       </c>
       <c r="J79" s="3">
-        <v>0.97121647930400301</v>
+        <v>0.97758051055526396</v>
       </c>
       <c r="K79" s="3">
         <v>0.97077699455370903</v>
@@ -4053,7 +3947,7 @@
       </c>
       <c r="M79" s="4">
         <f t="shared" si="54"/>
-        <v>0.96542039053213613</v>
+        <v>0.96752448526858836</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.35">
@@ -4062,7 +3956,7 @@
       </c>
       <c r="D80" s="4">
         <f>GEOMEAN(D76:D79)</f>
-        <v>1.0618041708519976</v>
+        <v>1.0500647527253353</v>
       </c>
       <c r="E80" s="4">
         <f t="shared" ref="E80" si="55">GEOMEAN(E76:E79)</f>
@@ -4074,14 +3968,14 @@
       </c>
       <c r="G80" s="4">
         <f>GEOMEAN(G76:G79)</f>
-        <v>1.0393989347860288</v>
+        <v>1.0355541625477376</v>
       </c>
       <c r="I80" s="2" t="s">
         <v>20</v>
       </c>
       <c r="J80" s="4">
         <f>GEOMEAN(J76:J79)</f>
-        <v>0.97920573901728636</v>
+        <v>0.97749594145057095</v>
       </c>
       <c r="K80" s="4">
         <f t="shared" ref="K80" si="57">GEOMEAN(K76:K79)</f>
@@ -4091,13 +3985,13 @@
         <f t="shared" ref="L80" si="58">GEOMEAN(L76:L79)</f>
         <v>0.96683901264654515</v>
       </c>
-      <c r="M80" s="4">
+      <c r="M80" s="5">
         <f>GEOMEAN(M76:M79)</f>
-        <v>0.97331949246072047</v>
+        <v>0.97275265589591842</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A81" s="5" t="s">
+      <c r="A81" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B81" s="2" t="s">
@@ -4116,7 +4010,7 @@
       <c r="L81" s="2"/>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A82" s="5"/>
+      <c r="A82" s="6"/>
       <c r="D82" s="1" t="s">
         <v>4</v>
       </c>
@@ -4129,7 +4023,7 @@
       <c r="L82" s="1"/>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A83" s="5"/>
+      <c r="A83" s="6"/>
       <c r="D83" s="2">
         <v>2</v>
       </c>
@@ -4156,7 +4050,7 @@
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A84" s="5"/>
+      <c r="A84" s="6"/>
       <c r="B84" s="1" t="s">
         <v>5</v>
       </c>
@@ -4164,7 +4058,7 @@
         <v>0</v>
       </c>
       <c r="D84" s="3">
-        <v>1.04918905115572</v>
+        <v>1.03997238752945</v>
       </c>
       <c r="E84" s="3">
         <v>1.0243397169178201</v>
@@ -4174,7 +4068,7 @@
       </c>
       <c r="G84" s="4">
         <f>GEOMEAN(D84:F84)</f>
-        <v>1.0312610980662456</v>
+        <v>1.0282324875225357</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>5</v>
@@ -4183,7 +4077,7 @@
         <v>0</v>
       </c>
       <c r="J84" s="3">
-        <v>0.96617793509254701</v>
+        <v>0.96619811294379898</v>
       </c>
       <c r="K84" s="3">
         <v>0.96374765394973705</v>
@@ -4193,17 +4087,17 @@
       </c>
       <c r="M84" s="4">
         <f>GEOMEAN(J84:L84)</f>
-        <v>0.96231731398504938</v>
+        <v>0.96232401301350723</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A85" s="5"/>
+      <c r="A85" s="6"/>
       <c r="B85" s="1"/>
       <c r="C85" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D85" s="3">
-        <v>1.05720963871041</v>
+        <v>1.0436541890019999</v>
       </c>
       <c r="E85" s="3">
         <v>1.02780806251239</v>
@@ -4213,14 +4107,14 @@
       </c>
       <c r="G85" s="4">
         <f t="shared" ref="G85:G87" si="59">GEOMEAN(D85:F85)</f>
-        <v>1.034447343782698</v>
+        <v>1.0300071140982399</v>
       </c>
       <c r="H85" s="1"/>
       <c r="I85" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J85" s="3">
-        <v>0.981766283622868</v>
+        <v>0.97868657703843198</v>
       </c>
       <c r="K85" s="3">
         <v>0.97808571687003298</v>
@@ -4230,17 +4124,17 @@
       </c>
       <c r="M85" s="4">
         <f t="shared" ref="M85:M87" si="60">GEOMEAN(J85:L85)</f>
-        <v>0.97884155054672783</v>
+        <v>0.97781696780031391</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A86" s="5"/>
+      <c r="A86" s="6"/>
       <c r="B86" s="1"/>
       <c r="C86" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D86" s="3">
-        <v>1.05377881022233</v>
+        <v>1.04727836690542</v>
       </c>
       <c r="E86" s="3">
         <v>1.0319375803820701</v>
@@ -4250,14 +4144,14 @@
       </c>
       <c r="G86" s="4">
         <f t="shared" si="59"/>
-        <v>1.0337443632101575</v>
+        <v>1.0316143584481661</v>
       </c>
       <c r="H86" s="1"/>
       <c r="I86" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J86" s="3">
-        <v>0.97454052166222505</v>
+        <v>0.97921554289505497</v>
       </c>
       <c r="K86" s="3">
         <v>0.97903950113632299</v>
@@ -4267,17 +4161,17 @@
       </c>
       <c r="M86" s="4">
         <f t="shared" si="60"/>
-        <v>0.97536462313530448</v>
+        <v>0.97692179397869938</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A87" s="5"/>
+      <c r="A87" s="6"/>
       <c r="B87" s="1"/>
       <c r="C87" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D87" s="3">
-        <v>1.0331121839133499</v>
+        <v>1.03565106580888</v>
       </c>
       <c r="E87" s="3">
         <v>1.02069229117426</v>
@@ -4287,14 +4181,14 @@
       </c>
       <c r="G87" s="4">
         <f t="shared" si="59"/>
-        <v>1.0122263025573053</v>
+        <v>1.0130548091289115</v>
       </c>
       <c r="H87" s="1"/>
       <c r="I87" s="2" t="s">
         <v>3</v>
       </c>
       <c r="J87" s="3">
-        <v>0.96384900163204301</v>
+        <v>0.97636843988674804</v>
       </c>
       <c r="K87" s="3">
         <v>0.97133494212655802</v>
@@ -4304,7 +4198,7 @@
       </c>
       <c r="M87" s="4">
         <f t="shared" si="60"/>
-        <v>0.96347062126196248</v>
+        <v>0.9676241970560252</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.35">
@@ -4313,7 +4207,7 @@
       </c>
       <c r="D88" s="4">
         <f>GEOMEAN(D84:D87)</f>
-        <v>1.0482815740655447</v>
+        <v>1.0416300599737374</v>
       </c>
       <c r="E88" s="4">
         <f t="shared" ref="E88" si="61">GEOMEAN(E84:E87)</f>
@@ -4325,14 +4219,14 @@
       </c>
       <c r="G88" s="4">
         <f>GEOMEAN(G84:G87)</f>
-        <v>1.027878895513928</v>
+        <v>1.0257002624588538</v>
       </c>
       <c r="I88" s="2" t="s">
         <v>20</v>
       </c>
       <c r="J88" s="4">
         <f>GEOMEAN(J84:J87)</f>
-        <v>0.97155755447212189</v>
+        <v>0.97510293132013648</v>
       </c>
       <c r="K88" s="4">
         <f t="shared" ref="K88" si="63">GEOMEAN(K84:K87)</f>
@@ -4342,13 +4236,13 @@
         <f t="shared" ref="L88" si="64">GEOMEAN(L84:L87)</f>
         <v>0.96534205495463998</v>
       </c>
-      <c r="M88" s="4">
+      <c r="M88" s="5">
         <f>GEOMEAN(M84:M87)</f>
-        <v>0.96997165432465027</v>
+        <v>0.9711500852646594</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A89" s="5" t="s">
+      <c r="A89" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B89" s="2" t="s">
@@ -4367,7 +4261,7 @@
       <c r="L89" s="2"/>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A90" s="5"/>
+      <c r="A90" s="6"/>
       <c r="D90" s="1" t="s">
         <v>4</v>
       </c>
@@ -4380,7 +4274,7 @@
       <c r="L90" s="1"/>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A91" s="5"/>
+      <c r="A91" s="6"/>
       <c r="D91" s="2">
         <v>2</v>
       </c>
@@ -4407,7 +4301,7 @@
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A92" s="5"/>
+      <c r="A92" s="6"/>
       <c r="B92" s="1" t="s">
         <v>5</v>
       </c>
@@ -4415,7 +4309,7 @@
         <v>0</v>
       </c>
       <c r="D92" s="3">
-        <v>1.04191466518083</v>
+        <v>1.03478466992846</v>
       </c>
       <c r="E92" s="3">
         <v>1.0185874630300999</v>
@@ -4425,7 +4319,7 @@
       </c>
       <c r="G92" s="4">
         <f>GEOMEAN(D92:F92)</f>
-        <v>1.0295013545331364</v>
+        <v>1.0271476277244687</v>
       </c>
       <c r="H92" s="1" t="s">
         <v>5</v>
@@ -4434,7 +4328,7 @@
         <v>0</v>
       </c>
       <c r="J92" s="3">
-        <v>0.96235863850553605</v>
+        <v>0.95976598349257303</v>
       </c>
       <c r="K92" s="3">
         <v>0.95388587731580099</v>
@@ -4444,17 +4338,17 @@
       </c>
       <c r="M92" s="4">
         <f>GEOMEAN(J92:L92)</f>
-        <v>0.95877197418714699</v>
+        <v>0.95791020239646796</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A93" s="5"/>
+      <c r="A93" s="6"/>
       <c r="B93" s="1"/>
       <c r="C93" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D93" s="3">
-        <v>1.04715659414977</v>
+        <v>1.0366546682945801</v>
       </c>
       <c r="E93" s="3">
         <v>1.0191612029375801</v>
@@ -4464,14 +4358,14 @@
       </c>
       <c r="G93" s="4">
         <f t="shared" ref="G93:G95" si="65">GEOMEAN(D93:F93)</f>
-        <v>1.0278212474339543</v>
+        <v>1.0243736925162708</v>
       </c>
       <c r="H93" s="1"/>
       <c r="I93" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J93" s="3">
-        <v>0.97328510956004799</v>
+        <v>0.97182610030346195</v>
       </c>
       <c r="K93" s="3">
         <v>0.96817232647983997</v>
@@ -4481,17 +4375,17 @@
       </c>
       <c r="M93" s="4">
         <f t="shared" ref="M93:M95" si="66">GEOMEAN(J93:L93)</f>
-        <v>0.97272786001530254</v>
+        <v>0.97224155896736386</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A94" s="5"/>
+      <c r="A94" s="6"/>
       <c r="B94" s="1"/>
       <c r="C94" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D94" s="3">
-        <v>1.04700382111408</v>
+        <v>1.0392230310199799</v>
       </c>
       <c r="E94" s="3">
         <v>1.01880351165478</v>
@@ -4501,14 +4395,14 @@
       </c>
       <c r="G94" s="4">
         <f t="shared" si="65"/>
-        <v>1.0286791538663198</v>
+        <v>1.0261246118129983</v>
       </c>
       <c r="H94" s="1"/>
       <c r="I94" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J94" s="3">
-        <v>0.96654889106271502</v>
+        <v>0.97161729992063395</v>
       </c>
       <c r="K94" s="3">
         <v>0.96680702864797896</v>
@@ -4518,17 +4412,17 @@
       </c>
       <c r="M94" s="4">
         <f t="shared" si="66"/>
-        <v>0.96866988749811656</v>
+        <v>0.97036011351210272</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A95" s="5"/>
+      <c r="A95" s="6"/>
       <c r="B95" s="1"/>
       <c r="C95" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D95" s="3">
-        <v>1.0285910329957799</v>
+        <v>1.02805804181204</v>
       </c>
       <c r="E95" s="3">
         <v>1.0101802048198401</v>
@@ -4538,14 +4432,14 @@
       </c>
       <c r="G95" s="4">
         <f t="shared" si="65"/>
-        <v>1.0107662482681545</v>
+        <v>1.0105916331681803</v>
       </c>
       <c r="H95" s="1"/>
       <c r="I95" s="2" t="s">
         <v>3</v>
       </c>
       <c r="J95" s="3">
-        <v>0.95516338079071095</v>
+        <v>0.96629024229542704</v>
       </c>
       <c r="K95" s="3">
         <v>0.95767947659487296</v>
@@ -4555,7 +4449,7 @@
       </c>
       <c r="M95" s="4">
         <f t="shared" si="66"/>
-        <v>0.9544333690059702</v>
+        <v>0.95812518951005499</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.35">
@@ -4564,7 +4458,7 @@
       </c>
       <c r="D96" s="4">
         <f>GEOMEAN(D92:D95)</f>
-        <v>1.0411389540548537</v>
+        <v>1.0346718245652979</v>
       </c>
       <c r="E96" s="4">
         <f t="shared" ref="E96" si="67">GEOMEAN(E92:E95)</f>
@@ -4576,14 +4470,14 @@
       </c>
       <c r="G96" s="4">
         <f>GEOMEAN(G92:G95)</f>
-        <v>1.0241623255952825</v>
+        <v>1.0220373604933215</v>
       </c>
       <c r="I96" s="2" t="s">
         <v>20</v>
       </c>
       <c r="J96" s="4">
         <f>GEOMEAN(J92:J95)</f>
-        <v>0.96431657088615275</v>
+        <v>0.96736236278058263</v>
       </c>
       <c r="K96" s="4">
         <f t="shared" ref="K96" si="69">GEOMEAN(K92:K95)</f>
@@ -4593,25 +4487,25 @@
         <f t="shared" ref="L96" si="70">GEOMEAN(L92:L95)</f>
         <v>0.96493748769712995</v>
       </c>
-      <c r="M96" s="4">
+      <c r="M96" s="5">
         <f>GEOMEAN(M92:M95)</f>
-        <v>0.96362270616725443</v>
+        <v>0.96463617334505225</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A89:A95"/>
+    <mergeCell ref="A49:A55"/>
+    <mergeCell ref="A65:A71"/>
+    <mergeCell ref="A73:A79"/>
+    <mergeCell ref="A81:A87"/>
+    <mergeCell ref="A57:A63"/>
     <mergeCell ref="A17:A23"/>
     <mergeCell ref="A25:A31"/>
     <mergeCell ref="A33:A39"/>
     <mergeCell ref="A41:A47"/>
     <mergeCell ref="A1:A7"/>
     <mergeCell ref="A9:A15"/>
-    <mergeCell ref="A89:A95"/>
-    <mergeCell ref="A49:A55"/>
-    <mergeCell ref="A65:A71"/>
-    <mergeCell ref="A73:A79"/>
-    <mergeCell ref="A81:A87"/>
-    <mergeCell ref="A57:A63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>